<commit_message>
Changed valve state reading functionality
</commit_message>
<xml_diff>
--- a/Measurements.xlsx
+++ b/Measurements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Perfusion_System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57826E83-BCEA-411B-A90D-5B4F259E38AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65795BF2-D92D-46F4-AE1E-C13AA897D955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -176,42 +176,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <font>
         <b val="0"/>
@@ -303,8 +268,8 @@
     <tableColumn id="3" xr3:uid="{42042122-A3C7-45DE-BE04-EE362424866A}" name="Raw_Low"/>
     <tableColumn id="4" xr3:uid="{38749820-830E-4531-9B07-60F99E376E35}" name="Empty_Weight"/>
     <tableColumn id="5" xr3:uid="{3C6786F6-9E55-48CD-86D5-85BF334A8548}" name="Final_Weight"/>
-    <tableColumn id="6" xr3:uid="{880A759E-940B-4C0C-99C2-58AD72247495}" name="Start_Time" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{1D3E761D-6183-43C4-A343-C4E44D78FD50}" name="End_Time" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{880A759E-940B-4C0C-99C2-58AD72247495}" name="Start_Time" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{1D3E761D-6183-43C4-A343-C4E44D78FD50}" name="End_Time" dataDxfId="5"/>
     <tableColumn id="8" xr3:uid="{75A5C027-3B36-48B6-86D0-E5E9FA3F4DCE}" name="Start_Volume (mL)"/>
     <tableColumn id="9" xr3:uid="{C4D2723B-1B01-441D-85D6-13310EAF7F91}" name="End_Volume (mL)"/>
     <tableColumn id="10" xr3:uid="{67DF149A-872D-49FA-A2C7-03C36BF4252C}" name="Flow_Rate (mL/Day)"/>
@@ -318,16 +283,16 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AFA1B13B-2067-4436-91E8-CE7B0EC89831}" name="Table2" displayName="Table2" ref="O3:R7" totalsRowShown="0">
   <autoFilter ref="O3:R7" xr:uid="{AFA1B13B-2067-4436-91E8-CE7B0EC89831}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{97463821-DEE2-4F42-AC00-A7A61AC07CE0}" name="Duration" dataDxfId="9">
+    <tableColumn id="1" xr3:uid="{97463821-DEE2-4F42-AC00-A7A61AC07CE0}" name="Duration" dataDxfId="4">
       <calculatedColumnFormula>H4-G4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{052C2071-850E-42F5-A26B-889DB58815C3}" name="Duration in Min" dataDxfId="8">
+    <tableColumn id="4" xr3:uid="{052C2071-850E-42F5-A26B-889DB58815C3}" name="Duration in Min" dataDxfId="3">
       <calculatedColumnFormula>O4</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{D45938C1-DA43-4572-97E8-35C0F3958EB1}" name="Volume by Syringe">
       <calculatedColumnFormula>I4-J4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{CE281EF5-AD90-4E03-8914-DD9A9D900FAD}" name="Volume by Weight" dataDxfId="7">
+    <tableColumn id="3" xr3:uid="{CE281EF5-AD90-4E03-8914-DD9A9D900FAD}" name="Volume by Weight" dataDxfId="2">
       <calculatedColumnFormula>(F4-E4)/0.9982</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -339,8 +304,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B419AA0D-6755-4C9D-BD52-00C6A845A2F0}" name="Table3" displayName="Table3" ref="U3:V11" totalsRowShown="0">
   <autoFilter ref="U3:V11" xr:uid="{B419AA0D-6755-4C9D-BD52-00C6A845A2F0}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{63D487F6-0EFF-42C3-90F0-E4DF35C983DE}" name="Flow-Rate" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{805730DE-BF4F-464F-9520-598D1BFA9242}" name="Accuracy" dataDxfId="5" dataCellStyle="Percent">
+    <tableColumn id="1" xr3:uid="{63D487F6-0EFF-42C3-90F0-E4DF35C983DE}" name="Flow-Rate" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{805730DE-BF4F-464F-9520-598D1BFA9242}" name="Accuracy" dataDxfId="0" dataCellStyle="Percent">
       <calculatedColumnFormula>(1-ABS(U4-K4)/K4)*100%</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -613,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:V14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1178,19 +1143,19 @@
         <v>25</v>
       </c>
       <c r="O12" s="3">
-        <f t="shared" ref="O12:O14" si="5">H12-G12</f>
+        <f t="shared" ref="O12" si="5">H12-G12</f>
         <v>9.7916666665696539E-2</v>
       </c>
       <c r="P12" s="4">
-        <f t="shared" ref="P12:P14" si="6">O12</f>
+        <f t="shared" ref="P12" si="6">O12</f>
         <v>9.7916666665696539E-2</v>
       </c>
       <c r="Q12" s="5">
-        <f t="shared" ref="Q12:Q14" si="7">I12-J12</f>
+        <f t="shared" ref="Q12" si="7">I12-J12</f>
         <v>2.4499999999999993</v>
       </c>
       <c r="R12" s="1">
-        <f t="shared" ref="R12:R14" si="8">(F12-E12)/0.9982</f>
+        <f t="shared" ref="R12" si="8">(F12-E12)/0.9982</f>
         <v>0</v>
       </c>
       <c r="U12" s="1">
@@ -1198,7 +1163,7 @@
         <v>25.021276595744673</v>
       </c>
       <c r="V12" s="7">
-        <f t="shared" ref="V12:V14" si="9">(1-ABS(U12-K12)/K12)*100%</f>
+        <f t="shared" ref="V12" si="9">(1-ABS(U12-K12)/K12)*100%</f>
         <v>0.99914893617021305</v>
       </c>
     </row>
@@ -1222,54 +1187,100 @@
         <v>45870.459027777775</v>
       </c>
       <c r="H13" s="6">
-        <v>45870.556944444441</v>
+        <v>45870.604166666664</v>
       </c>
       <c r="I13">
         <v>9.6</v>
       </c>
       <c r="J13">
-        <v>7.15</v>
+        <v>6</v>
       </c>
       <c r="K13">
         <v>25</v>
       </c>
       <c r="O13" s="3">
         <f t="shared" ref="O13" si="10">H13-G13</f>
-        <v>9.7916666665696539E-2</v>
+        <v>0.14513888888905058</v>
       </c>
       <c r="P13" s="4">
         <f t="shared" ref="P13" si="11">O13</f>
-        <v>9.7916666665696539E-2</v>
+        <v>0.14513888888905058</v>
       </c>
       <c r="Q13" s="5">
         <f t="shared" ref="Q13" si="12">I13-J13</f>
-        <v>2.4499999999999993</v>
+        <v>3.5999999999999996</v>
       </c>
       <c r="R13" s="1">
         <f t="shared" ref="R13" si="13">(F13-E13)/0.9982</f>
         <v>0</v>
       </c>
       <c r="U13" s="1">
-        <f>Q13*1440/141</f>
-        <v>25.021276595744673</v>
+        <f>Q13*1440/209</f>
+        <v>24.803827751196167</v>
       </c>
       <c r="V13" s="7">
         <f t="shared" ref="V13" si="14">(1-ABS(U13-K13)/K13)*100%</f>
-        <v>0.99914893617021305</v>
+        <v>0.99215311004784668</v>
       </c>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="1"/>
-      <c r="U14" s="1"/>
-      <c r="V14" s="7"/>
+      <c r="B14">
+        <v>11</v>
+      </c>
+      <c r="C14">
+        <v>290</v>
+      </c>
+      <c r="D14">
+        <v>163</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14" s="6">
+        <v>45870.60833333333</v>
+      </c>
+      <c r="H14" s="6">
+        <v>45870.703472222223</v>
+      </c>
+      <c r="I14">
+        <v>6</v>
+      </c>
+      <c r="J14">
+        <v>5.48</v>
+      </c>
+      <c r="K14">
+        <v>5</v>
+      </c>
+      <c r="O14" s="3">
+        <f t="shared" ref="O14" si="15">H14-G14</f>
+        <v>9.5138888893416151E-2</v>
+      </c>
+      <c r="P14" s="4">
+        <f t="shared" ref="P14" si="16">O14</f>
+        <v>9.5138888893416151E-2</v>
+      </c>
+      <c r="Q14" s="5">
+        <f t="shared" ref="Q14" si="17">I14-J14</f>
+        <v>0.51999999999999957</v>
+      </c>
+      <c r="R14" s="1">
+        <f t="shared" ref="R14" si="18">(F14-E14)/0.9982</f>
+        <v>0</v>
+      </c>
+      <c r="U14" s="1">
+        <f>Q14*1440/137</f>
+        <v>5.4656934306569296</v>
+      </c>
+      <c r="V14" s="7">
+        <f t="shared" ref="V14" si="19">(1-ABS(U14-K14)/K14)*100%</f>
+        <v>0.90686131386861413</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="V4:V13">
+  <conditionalFormatting sqref="V4:V14">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
New UI added to Dashboard_2
</commit_message>
<xml_diff>
--- a/Measurements.xlsx
+++ b/Measurements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Perfusion_System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65795BF2-D92D-46F4-AE1E-C13AA897D955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4DB786-4258-4AEC-B0F6-B9C89C1BB575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -260,8 +260,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5A39537A-AD85-40E4-8132-CD746B4A4B1E}" name="Table1" displayName="Table1" ref="B3:L14" totalsRowShown="0">
-  <autoFilter ref="B3:L14" xr:uid="{5A39537A-AD85-40E4-8132-CD746B4A4B1E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5A39537A-AD85-40E4-8132-CD746B4A4B1E}" name="Table1" displayName="Table1" ref="B3:L16" totalsRowShown="0">
+  <autoFilter ref="B3:L16" xr:uid="{5A39537A-AD85-40E4-8132-CD746B4A4B1E}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{7F49C8BC-1009-4421-9279-20BA630C3F5B}" name="Index"/>
     <tableColumn id="2" xr3:uid="{5E47D918-C96A-47BF-882D-1F6F0C3B3A06}" name="Raw_High"/>
@@ -576,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:V14"/>
+  <dimension ref="B3:V16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+      <selection activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1279,8 +1279,68 @@
         <v>0.90686131386861413</v>
       </c>
     </row>
+    <row r="15" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B15">
+        <v>12</v>
+      </c>
+      <c r="C15">
+        <v>286</v>
+      </c>
+      <c r="D15">
+        <v>159</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15" s="6">
+        <v>45876.647916666669</v>
+      </c>
+      <c r="H15" s="6">
+        <v>45877.597222222219</v>
+      </c>
+      <c r="I15">
+        <v>11.95</v>
+      </c>
+      <c r="J15">
+        <v>9.5500000000000007</v>
+      </c>
+      <c r="K15">
+        <v>2.5</v>
+      </c>
+      <c r="O15" s="3">
+        <f t="shared" ref="O15" si="20">H15-G15</f>
+        <v>0.94930555555038154</v>
+      </c>
+      <c r="P15" s="4">
+        <f t="shared" ref="P15" si="21">O15</f>
+        <v>0.94930555555038154</v>
+      </c>
+      <c r="Q15" s="5">
+        <f t="shared" ref="Q15" si="22">I15-J15</f>
+        <v>2.3999999999999986</v>
+      </c>
+      <c r="R15" s="1">
+        <f t="shared" ref="R15" si="23">(F15-E15)/0.9982</f>
+        <v>0</v>
+      </c>
+      <c r="U15" s="1">
+        <f>Q15*1440/1367</f>
+        <v>2.5281638624725664</v>
+      </c>
+      <c r="V15" s="7">
+        <f t="shared" ref="V15" si="24">(1-ABS(U15-K15)/K15)*100%</f>
+        <v>0.98873445501097346</v>
+      </c>
+    </row>
+    <row r="16" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="V4:V14">
+  <conditionalFormatting sqref="V4:V15">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Minor bug fixes and new Measurements added.
</commit_message>
<xml_diff>
--- a/Measurements.xlsx
+++ b/Measurements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Perfusion_System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4DB786-4258-4AEC-B0F6-B9C89C1BB575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2B1F05-D106-4828-AE04-58EB007B52D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -103,7 +103,7 @@
     <numFmt numFmtId="166" formatCode="[m]"/>
     <numFmt numFmtId="167" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,6 +130,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -162,7 +167,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -171,6 +176,9 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -260,8 +268,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5A39537A-AD85-40E4-8132-CD746B4A4B1E}" name="Table1" displayName="Table1" ref="B3:L16" totalsRowShown="0">
-  <autoFilter ref="B3:L16" xr:uid="{5A39537A-AD85-40E4-8132-CD746B4A4B1E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5A39537A-AD85-40E4-8132-CD746B4A4B1E}" name="Table1" displayName="Table1" ref="B3:L18" totalsRowShown="0">
+  <autoFilter ref="B3:L18" xr:uid="{5A39537A-AD85-40E4-8132-CD746B4A4B1E}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{7F49C8BC-1009-4421-9279-20BA630C3F5B}" name="Index"/>
     <tableColumn id="2" xr3:uid="{5E47D918-C96A-47BF-882D-1F6F0C3B3A06}" name="Raw_High"/>
@@ -576,10 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:V16"/>
+  <dimension ref="B3:V31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V16" sqref="V16"/>
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1336,11 +1344,162 @@
       </c>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
+      <c r="B16">
+        <v>13</v>
+      </c>
+      <c r="C16">
+        <v>286</v>
+      </c>
+      <c r="D16">
+        <v>159</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16" s="6">
+        <v>45876.647916666669</v>
+      </c>
+      <c r="H16" s="6">
+        <v>45880.591666666667</v>
+      </c>
+      <c r="I16">
+        <v>11.95</v>
+      </c>
+      <c r="J16">
+        <v>1.5</v>
+      </c>
+      <c r="K16">
+        <v>2.5</v>
+      </c>
+      <c r="O16" s="3">
+        <f t="shared" ref="O16" si="25">H16-G16</f>
+        <v>3.9437499999985448</v>
+      </c>
+      <c r="P16" s="4">
+        <f t="shared" ref="P16" si="26">O16</f>
+        <v>3.9437499999985448</v>
+      </c>
+      <c r="Q16" s="5">
+        <f t="shared" ref="Q16" si="27">I16-J16</f>
+        <v>10.45</v>
+      </c>
+      <c r="R16" s="1">
+        <f t="shared" ref="R16" si="28">(F16-E16)/0.9982</f>
+        <v>0</v>
+      </c>
+      <c r="U16" s="1">
+        <f>Q16*1440/5679</f>
+        <v>2.6497622820919173</v>
+      </c>
+      <c r="V16" s="7">
+        <f t="shared" ref="V16" si="29">(1-ABS(U16-K16)/K16)*100%</f>
+        <v>0.94009508716323309</v>
+      </c>
+    </row>
+    <row r="17" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B17">
+        <v>14</v>
+      </c>
+      <c r="C17">
+        <v>286</v>
+      </c>
+      <c r="D17">
+        <v>159</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17" s="6">
+        <v>45877.597222222219</v>
+      </c>
+      <c r="H17" s="6">
+        <v>45880.591666666667</v>
+      </c>
+      <c r="I17">
+        <v>9.5500000000000007</v>
+      </c>
+      <c r="J17">
+        <v>1.5</v>
+      </c>
+      <c r="K17">
+        <v>2.5</v>
+      </c>
+      <c r="O17" s="3">
+        <f t="shared" ref="O17" si="30">H17-G17</f>
+        <v>2.9944444444481633</v>
+      </c>
+      <c r="P17" s="4">
+        <f t="shared" ref="P17" si="31">O17</f>
+        <v>2.9944444444481633</v>
+      </c>
+      <c r="Q17" s="5">
+        <f t="shared" ref="Q17" si="32">I17-J17</f>
+        <v>8.0500000000000007</v>
+      </c>
+      <c r="R17" s="1">
+        <f t="shared" ref="R17" si="33">(F17-E17)/0.9982</f>
+        <v>0</v>
+      </c>
+      <c r="U17" s="1">
+        <f>Q17*1440/4312</f>
+        <v>2.6883116883116887</v>
+      </c>
+      <c r="V17" s="7">
+        <f t="shared" ref="V17" si="34">(1-ABS(U17-K17)/K17)*100%</f>
+        <v>0.92467532467532454</v>
+      </c>
+    </row>
+    <row r="18" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+    </row>
+    <row r="28" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="H28" s="8">
+        <v>65.773633770000004</v>
+      </c>
+      <c r="I28">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="J28">
+        <f>H28/I28</f>
+        <v>28.597232073913048</v>
+      </c>
+    </row>
+    <row r="29" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="H29" s="8">
+        <v>80.890960000000007</v>
+      </c>
+      <c r="I29">
+        <v>2.69</v>
+      </c>
+      <c r="J29">
+        <f>H29/I29</f>
+        <v>30.070988847583646</v>
+      </c>
+    </row>
+    <row r="30" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="I30">
+        <v>2.5</v>
+      </c>
+      <c r="J30">
+        <f>(J28+J29)/2</f>
+        <v>29.334110460748349</v>
+      </c>
+    </row>
+    <row r="31" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="J31">
+        <f>J30*I30</f>
+        <v>73.335276151870872</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="V4:V15">
+  <conditionalFormatting sqref="V4:V17">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
New 3D files and Measurements added.
</commit_message>
<xml_diff>
--- a/Measurements.xlsx
+++ b/Measurements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Perfusion_System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2B1F05-D106-4828-AE04-58EB007B52D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E81EA3-F260-41A5-A802-1D5945363D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Raw_High</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Expected Vol for Perfusion</t>
   </si>
 </sst>
 </file>
@@ -184,7 +187,10 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -268,16 +274,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5A39537A-AD85-40E4-8132-CD746B4A4B1E}" name="Table1" displayName="Table1" ref="B3:L18" totalsRowShown="0">
-  <autoFilter ref="B3:L18" xr:uid="{5A39537A-AD85-40E4-8132-CD746B4A4B1E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5A39537A-AD85-40E4-8132-CD746B4A4B1E}" name="Table1" displayName="Table1" ref="B3:L19" totalsRowShown="0">
+  <autoFilter ref="B3:L19" xr:uid="{5A39537A-AD85-40E4-8132-CD746B4A4B1E}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{7F49C8BC-1009-4421-9279-20BA630C3F5B}" name="Index"/>
     <tableColumn id="2" xr3:uid="{5E47D918-C96A-47BF-882D-1F6F0C3B3A06}" name="Raw_High"/>
     <tableColumn id="3" xr3:uid="{42042122-A3C7-45DE-BE04-EE362424866A}" name="Raw_Low"/>
     <tableColumn id="4" xr3:uid="{38749820-830E-4531-9B07-60F99E376E35}" name="Empty_Weight"/>
     <tableColumn id="5" xr3:uid="{3C6786F6-9E55-48CD-86D5-85BF334A8548}" name="Final_Weight"/>
-    <tableColumn id="6" xr3:uid="{880A759E-940B-4C0C-99C2-58AD72247495}" name="Start_Time" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{1D3E761D-6183-43C4-A343-C4E44D78FD50}" name="End_Time" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{880A759E-940B-4C0C-99C2-58AD72247495}" name="Start_Time" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{1D3E761D-6183-43C4-A343-C4E44D78FD50}" name="End_Time" dataDxfId="6"/>
     <tableColumn id="8" xr3:uid="{75A5C027-3B36-48B6-86D0-E5E9FA3F4DCE}" name="Start_Volume (mL)"/>
     <tableColumn id="9" xr3:uid="{C4D2723B-1B01-441D-85D6-13310EAF7F91}" name="End_Volume (mL)"/>
     <tableColumn id="10" xr3:uid="{67DF149A-872D-49FA-A2C7-03C36BF4252C}" name="Flow_Rate (mL/Day)"/>
@@ -288,23 +294,26 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AFA1B13B-2067-4436-91E8-CE7B0EC89831}" name="Table2" displayName="Table2" ref="O3:R7" totalsRowShown="0">
-  <autoFilter ref="O3:R7" xr:uid="{AFA1B13B-2067-4436-91E8-CE7B0EC89831}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{97463821-DEE2-4F42-AC00-A7A61AC07CE0}" name="Duration" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AFA1B13B-2067-4436-91E8-CE7B0EC89831}" name="Table2" displayName="Table2" ref="O3:S19" totalsRowShown="0">
+  <autoFilter ref="O3:S19" xr:uid="{AFA1B13B-2067-4436-91E8-CE7B0EC89831}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{97463821-DEE2-4F42-AC00-A7A61AC07CE0}" name="Duration" dataDxfId="5">
       <calculatedColumnFormula>H4-G4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{052C2071-850E-42F5-A26B-889DB58815C3}" name="Duration in Min" dataDxfId="3">
+    <tableColumn id="4" xr3:uid="{052C2071-850E-42F5-A26B-889DB58815C3}" name="Duration in Min" dataDxfId="4">
       <calculatedColumnFormula>O4</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{D45938C1-DA43-4572-97E8-35C0F3958EB1}" name="Volume by Syringe">
       <calculatedColumnFormula>I4-J4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{CE281EF5-AD90-4E03-8914-DD9A9D900FAD}" name="Volume by Weight" dataDxfId="2">
+    <tableColumn id="3" xr3:uid="{CE281EF5-AD90-4E03-8914-DD9A9D900FAD}" name="Volume by Weight" dataDxfId="3">
       <calculatedColumnFormula>(F4-E4)/0.9982</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="5" xr3:uid="{9AD10D29-13FB-4A61-B0DA-D4754470DC60}" name="Expected Vol for Perfusion" dataDxfId="0">
+      <calculatedColumnFormula>K4*P4</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -312,8 +321,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B419AA0D-6755-4C9D-BD52-00C6A845A2F0}" name="Table3" displayName="Table3" ref="U3:V11" totalsRowShown="0">
   <autoFilter ref="U3:V11" xr:uid="{B419AA0D-6755-4C9D-BD52-00C6A845A2F0}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{63D487F6-0EFF-42C3-90F0-E4DF35C983DE}" name="Flow-Rate" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{805730DE-BF4F-464F-9520-598D1BFA9242}" name="Accuracy" dataDxfId="0" dataCellStyle="Percent">
+    <tableColumn id="1" xr3:uid="{63D487F6-0EFF-42C3-90F0-E4DF35C983DE}" name="Flow-Rate" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{805730DE-BF4F-464F-9520-598D1BFA9242}" name="Accuracy" dataDxfId="1" dataCellStyle="Percent">
       <calculatedColumnFormula>(1-ABS(U4-K4)/K4)*100%</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -584,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:V31"/>
+  <dimension ref="B3:W45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
+      <selection activeCell="R44" sqref="R44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -603,10 +612,10 @@
     <col min="11" max="11" width="20.6328125" customWidth="1"/>
     <col min="12" max="12" width="23.453125" customWidth="1"/>
     <col min="15" max="15" width="12.453125" customWidth="1"/>
-    <col min="16" max="16" width="16.7265625" customWidth="1"/>
-    <col min="17" max="17" width="19.54296875" customWidth="1"/>
+    <col min="16" max="16" width="16.26953125" customWidth="1"/>
+    <col min="17" max="17" width="18.54296875" customWidth="1"/>
     <col min="18" max="18" width="19.7265625" customWidth="1"/>
-    <col min="19" max="19" width="19.81640625" customWidth="1"/>
+    <col min="19" max="19" width="25.36328125" customWidth="1"/>
     <col min="21" max="21" width="11.54296875" customWidth="1"/>
     <col min="22" max="22" width="10.6328125" customWidth="1"/>
   </cols>
@@ -657,6 +666,9 @@
       <c r="R3" t="s">
         <v>11</v>
       </c>
+      <c r="S3" t="s">
+        <v>19</v>
+      </c>
       <c r="U3" t="s">
         <v>16</v>
       </c>
@@ -713,6 +725,10 @@
       <c r="R4" s="1">
         <f t="shared" ref="R4:R11" si="3">(F4-E4)/0.9982</f>
         <v>1.0018032458425166</v>
+      </c>
+      <c r="S4" s="5">
+        <f t="shared" ref="S4:S18" si="4">K4*P4</f>
+        <v>1.3107638888868678</v>
       </c>
       <c r="T4" s="5"/>
       <c r="U4" s="1">
@@ -771,12 +787,16 @@
         <f t="shared" si="3"/>
         <v>0.30054097375275479</v>
       </c>
+      <c r="S5" s="5">
+        <f t="shared" si="4"/>
+        <v>0.42881944444161491</v>
+      </c>
       <c r="U5" s="1">
         <f>Q5*1440/247</f>
         <v>2.3319838056680182</v>
       </c>
       <c r="V5" s="7">
-        <f t="shared" ref="V5:V11" si="4">(1-ABS(U5-K5)/K5)*100%</f>
+        <f t="shared" ref="V5:V11" si="5">(1-ABS(U5-K5)/K5)*100%</f>
         <v>0.93279352226720724</v>
       </c>
     </row>
@@ -827,12 +847,16 @@
         <f t="shared" si="3"/>
         <v>1.4526147064716493</v>
       </c>
+      <c r="S6" s="5">
+        <f t="shared" si="4"/>
+        <v>1.8454861111058563</v>
+      </c>
       <c r="U6" s="1">
         <f>Q6*1440/1052</f>
         <v>2.2585551330798483</v>
       </c>
       <c r="V6" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.90342205323193936</v>
       </c>
     </row>
@@ -883,12 +907,16 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+      <c r="S7" s="5">
+        <f t="shared" si="4"/>
+        <v>1.180555555401952</v>
+      </c>
       <c r="U7" s="1">
         <f>Q7*1440/68</f>
         <v>21.176470588235293</v>
       </c>
       <c r="V7" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.84705882352941175</v>
       </c>
     </row>
@@ -942,12 +970,16 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+      <c r="S8" s="5">
+        <f t="shared" si="4"/>
+        <v>1.0590277777737356</v>
+      </c>
       <c r="U8" s="1">
         <f>Q8*1440/61</f>
         <v>22.426229508196727</v>
       </c>
       <c r="V8" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.89704918032786907</v>
       </c>
     </row>
@@ -998,12 +1030,16 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+      <c r="S9" s="5">
+        <f t="shared" si="4"/>
+        <v>2.3090277776645962</v>
+      </c>
       <c r="U9" s="1">
         <f>Q9*1440/133</f>
         <v>27.609022556390975</v>
       </c>
       <c r="V9" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.89563909774436101</v>
       </c>
     </row>
@@ -1054,12 +1090,16 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+      <c r="S10" s="5">
+        <f t="shared" si="4"/>
+        <v>1.7881944444525288</v>
+      </c>
       <c r="U10" s="1">
         <f>Q10*1440/103</f>
         <v>27.961165048543688</v>
       </c>
       <c r="V10" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.8815533980582525</v>
       </c>
     </row>
@@ -1110,12 +1150,16 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+      <c r="S11" s="5">
+        <f t="shared" si="4"/>
+        <v>1.7482638888941437</v>
+      </c>
       <c r="U11" s="1">
         <f>Q11*1440/1007</f>
         <v>2.5024826216484608</v>
       </c>
       <c r="V11" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.99900695134061568</v>
       </c>
     </row>
@@ -1151,27 +1195,31 @@
         <v>25</v>
       </c>
       <c r="O12" s="3">
-        <f t="shared" ref="O12" si="5">H12-G12</f>
+        <f t="shared" ref="O12" si="6">H12-G12</f>
         <v>9.7916666665696539E-2</v>
       </c>
       <c r="P12" s="4">
-        <f t="shared" ref="P12" si="6">O12</f>
+        <f t="shared" ref="P12" si="7">O12</f>
         <v>9.7916666665696539E-2</v>
       </c>
       <c r="Q12" s="5">
-        <f t="shared" ref="Q12" si="7">I12-J12</f>
+        <f t="shared" ref="Q12" si="8">I12-J12</f>
         <v>2.4499999999999993</v>
       </c>
       <c r="R12" s="1">
-        <f t="shared" ref="R12" si="8">(F12-E12)/0.9982</f>
-        <v>0</v>
+        <f t="shared" ref="R12" si="9">(F12-E12)/0.9982</f>
+        <v>0</v>
+      </c>
+      <c r="S12" s="5">
+        <f t="shared" si="4"/>
+        <v>2.4479166666424135</v>
       </c>
       <c r="U12" s="1">
         <f>Q12*1440/141</f>
         <v>25.021276595744673</v>
       </c>
       <c r="V12" s="7">
-        <f t="shared" ref="V12" si="9">(1-ABS(U12-K12)/K12)*100%</f>
+        <f t="shared" ref="V12" si="10">(1-ABS(U12-K12)/K12)*100%</f>
         <v>0.99914893617021305</v>
       </c>
     </row>
@@ -1207,27 +1255,31 @@
         <v>25</v>
       </c>
       <c r="O13" s="3">
-        <f t="shared" ref="O13" si="10">H13-G13</f>
+        <f t="shared" ref="O13" si="11">H13-G13</f>
         <v>0.14513888888905058</v>
       </c>
       <c r="P13" s="4">
-        <f t="shared" ref="P13" si="11">O13</f>
+        <f t="shared" ref="P13" si="12">O13</f>
         <v>0.14513888888905058</v>
       </c>
       <c r="Q13" s="5">
-        <f t="shared" ref="Q13" si="12">I13-J13</f>
+        <f t="shared" ref="Q13" si="13">I13-J13</f>
         <v>3.5999999999999996</v>
       </c>
       <c r="R13" s="1">
-        <f t="shared" ref="R13" si="13">(F13-E13)/0.9982</f>
-        <v>0</v>
+        <f t="shared" ref="R13" si="14">(F13-E13)/0.9982</f>
+        <v>0</v>
+      </c>
+      <c r="S13" s="5">
+        <f t="shared" si="4"/>
+        <v>3.6284722222262644</v>
       </c>
       <c r="U13" s="1">
         <f>Q13*1440/209</f>
         <v>24.803827751196167</v>
       </c>
       <c r="V13" s="7">
-        <f t="shared" ref="V13" si="14">(1-ABS(U13-K13)/K13)*100%</f>
+        <f t="shared" ref="V13" si="15">(1-ABS(U13-K13)/K13)*100%</f>
         <v>0.99215311004784668</v>
       </c>
     </row>
@@ -1263,27 +1315,31 @@
         <v>5</v>
       </c>
       <c r="O14" s="3">
-        <f t="shared" ref="O14" si="15">H14-G14</f>
+        <f t="shared" ref="O14" si="16">H14-G14</f>
         <v>9.5138888893416151E-2</v>
       </c>
       <c r="P14" s="4">
-        <f t="shared" ref="P14" si="16">O14</f>
+        <f t="shared" ref="P14" si="17">O14</f>
         <v>9.5138888893416151E-2</v>
       </c>
       <c r="Q14" s="5">
-        <f t="shared" ref="Q14" si="17">I14-J14</f>
+        <f t="shared" ref="Q14" si="18">I14-J14</f>
         <v>0.51999999999999957</v>
       </c>
       <c r="R14" s="1">
-        <f t="shared" ref="R14" si="18">(F14-E14)/0.9982</f>
-        <v>0</v>
+        <f t="shared" ref="R14" si="19">(F14-E14)/0.9982</f>
+        <v>0</v>
+      </c>
+      <c r="S14" s="5">
+        <f t="shared" si="4"/>
+        <v>0.47569444446708076</v>
       </c>
       <c r="U14" s="1">
         <f>Q14*1440/137</f>
         <v>5.4656934306569296</v>
       </c>
       <c r="V14" s="7">
-        <f t="shared" ref="V14" si="19">(1-ABS(U14-K14)/K14)*100%</f>
+        <f t="shared" ref="V14" si="20">(1-ABS(U14-K14)/K14)*100%</f>
         <v>0.90686131386861413</v>
       </c>
     </row>
@@ -1319,27 +1375,31 @@
         <v>2.5</v>
       </c>
       <c r="O15" s="3">
-        <f t="shared" ref="O15" si="20">H15-G15</f>
+        <f t="shared" ref="O15" si="21">H15-G15</f>
         <v>0.94930555555038154</v>
       </c>
       <c r="P15" s="4">
-        <f t="shared" ref="P15" si="21">O15</f>
+        <f t="shared" ref="P15" si="22">O15</f>
         <v>0.94930555555038154</v>
       </c>
       <c r="Q15" s="5">
-        <f t="shared" ref="Q15" si="22">I15-J15</f>
+        <f t="shared" ref="Q15" si="23">I15-J15</f>
         <v>2.3999999999999986</v>
       </c>
       <c r="R15" s="1">
-        <f t="shared" ref="R15" si="23">(F15-E15)/0.9982</f>
-        <v>0</v>
+        <f t="shared" ref="R15" si="24">(F15-E15)/0.9982</f>
+        <v>0</v>
+      </c>
+      <c r="S15" s="5">
+        <f t="shared" si="4"/>
+        <v>2.3732638888759539</v>
       </c>
       <c r="U15" s="1">
         <f>Q15*1440/1367</f>
         <v>2.5281638624725664</v>
       </c>
       <c r="V15" s="7">
-        <f t="shared" ref="V15" si="24">(1-ABS(U15-K15)/K15)*100%</f>
+        <f t="shared" ref="V15" si="25">(1-ABS(U15-K15)/K15)*100%</f>
         <v>0.98873445501097346</v>
       </c>
     </row>
@@ -1375,31 +1435,35 @@
         <v>2.5</v>
       </c>
       <c r="O16" s="3">
-        <f t="shared" ref="O16" si="25">H16-G16</f>
+        <f t="shared" ref="O16" si="26">H16-G16</f>
         <v>3.9437499999985448</v>
       </c>
       <c r="P16" s="4">
-        <f t="shared" ref="P16" si="26">O16</f>
+        <f t="shared" ref="P16" si="27">O16</f>
         <v>3.9437499999985448</v>
       </c>
       <c r="Q16" s="5">
-        <f t="shared" ref="Q16" si="27">I16-J16</f>
+        <f t="shared" ref="Q16" si="28">I16-J16</f>
         <v>10.45</v>
       </c>
       <c r="R16" s="1">
-        <f t="shared" ref="R16" si="28">(F16-E16)/0.9982</f>
-        <v>0</v>
+        <f t="shared" ref="R16" si="29">(F16-E16)/0.9982</f>
+        <v>0</v>
+      </c>
+      <c r="S16" s="5">
+        <f t="shared" si="4"/>
+        <v>9.859374999996362</v>
       </c>
       <c r="U16" s="1">
         <f>Q16*1440/5679</f>
         <v>2.6497622820919173</v>
       </c>
       <c r="V16" s="7">
-        <f t="shared" ref="V16" si="29">(1-ABS(U16-K16)/K16)*100%</f>
+        <f t="shared" ref="V16" si="30">(1-ABS(U16-K16)/K16)*100%</f>
         <v>0.94009508716323309</v>
       </c>
     </row>
-    <row r="17" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B17">
         <v>14</v>
       </c>
@@ -1431,35 +1495,166 @@
         <v>2.5</v>
       </c>
       <c r="O17" s="3">
-        <f t="shared" ref="O17" si="30">H17-G17</f>
+        <f t="shared" ref="O17" si="31">H17-G17</f>
         <v>2.9944444444481633</v>
       </c>
       <c r="P17" s="4">
-        <f t="shared" ref="P17" si="31">O17</f>
+        <f t="shared" ref="P17" si="32">O17</f>
         <v>2.9944444444481633</v>
       </c>
       <c r="Q17" s="5">
-        <f t="shared" ref="Q17" si="32">I17-J17</f>
+        <f t="shared" ref="Q17" si="33">I17-J17</f>
         <v>8.0500000000000007</v>
       </c>
       <c r="R17" s="1">
-        <f t="shared" ref="R17" si="33">(F17-E17)/0.9982</f>
-        <v>0</v>
+        <f t="shared" ref="R17" si="34">(F17-E17)/0.9982</f>
+        <v>0</v>
+      </c>
+      <c r="S17" s="5">
+        <f t="shared" si="4"/>
+        <v>7.4861111111204082</v>
       </c>
       <c r="U17" s="1">
         <f>Q17*1440/4312</f>
         <v>2.6883116883116887</v>
       </c>
       <c r="V17" s="7">
-        <f t="shared" ref="V17" si="34">(1-ABS(U17-K17)/K17)*100%</f>
+        <f t="shared" ref="V17" si="35">(1-ABS(U17-K17)/K17)*100%</f>
         <v>0.92467532467532454</v>
       </c>
     </row>
-    <row r="18" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-    </row>
-    <row r="28" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="B18">
+        <v>15</v>
+      </c>
+      <c r="C18">
+        <v>286</v>
+      </c>
+      <c r="D18">
+        <v>159</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18" s="6">
+        <v>45880.736805555556</v>
+      </c>
+      <c r="H18" s="6">
+        <v>45881.38958333333</v>
+      </c>
+      <c r="I18">
+        <v>11.65</v>
+      </c>
+      <c r="J18">
+        <v>10.1</v>
+      </c>
+      <c r="K18">
+        <v>2.5</v>
+      </c>
+      <c r="O18" s="3">
+        <f t="shared" ref="O18" si="36">H18-G18</f>
+        <v>0.65277777777373558</v>
+      </c>
+      <c r="P18" s="4">
+        <f t="shared" ref="P18" si="37">O18</f>
+        <v>0.65277777777373558</v>
+      </c>
+      <c r="Q18" s="5">
+        <f t="shared" ref="Q18" si="38">I18-J18</f>
+        <v>1.5500000000000007</v>
+      </c>
+      <c r="R18" s="1">
+        <f t="shared" ref="R18" si="39">(F18-E18)/0.9982</f>
+        <v>0</v>
+      </c>
+      <c r="S18" s="5">
+        <f t="shared" si="4"/>
+        <v>1.6319444444343389</v>
+      </c>
+      <c r="U18" s="1">
+        <f>Q18*1440/940</f>
+        <v>2.374468085106384</v>
+      </c>
+      <c r="V18" s="7">
+        <f t="shared" ref="V18" si="40">(1-ABS(U18-K18)/K18)*100%</f>
+        <v>0.94978723404255361</v>
+      </c>
+    </row>
+    <row r="19" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="B19">
+        <v>16</v>
+      </c>
+      <c r="C19">
+        <v>286</v>
+      </c>
+      <c r="D19">
+        <v>159</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19" s="6">
+        <v>45880.736805555556</v>
+      </c>
+      <c r="H19" s="6">
+        <v>45882.484027777777</v>
+      </c>
+      <c r="I19">
+        <v>11.65</v>
+      </c>
+      <c r="J19">
+        <v>7.5</v>
+      </c>
+      <c r="K19">
+        <v>2.5</v>
+      </c>
+      <c r="O19" s="3">
+        <f t="shared" ref="O19" si="41">H19-G19</f>
+        <v>1.7472222222204437</v>
+      </c>
+      <c r="P19" s="4">
+        <f t="shared" ref="P19" si="42">O19</f>
+        <v>1.7472222222204437</v>
+      </c>
+      <c r="Q19" s="5">
+        <f t="shared" ref="Q19" si="43">I19-J19</f>
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="R19" s="1">
+        <f t="shared" ref="R19" si="44">(F19-E19)/0.9982</f>
+        <v>0</v>
+      </c>
+      <c r="S19" s="5">
+        <f>K19*P19</f>
+        <v>4.3680555555511091</v>
+      </c>
+      <c r="U19" s="1">
+        <f>Q19*1440/2516</f>
+        <v>2.375198728139905</v>
+      </c>
+      <c r="V19" s="7">
+        <f t="shared" ref="V19" si="45">(1-ABS(U19-K19)/K19)*100%</f>
+        <v>0.95007949125596203</v>
+      </c>
+    </row>
+    <row r="27" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="L27">
+        <v>65.77</v>
+      </c>
+      <c r="P27">
+        <v>80.89</v>
+      </c>
+      <c r="T27">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="2:23" x14ac:dyDescent="0.35">
       <c r="H28" s="8">
         <v>65.773633770000004</v>
       </c>
@@ -1470,8 +1665,47 @@
         <f>H28/I28</f>
         <v>28.597232073913048</v>
       </c>
-    </row>
-    <row r="29" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="L28">
+        <v>247</v>
+      </c>
+      <c r="M28">
+        <v>0.4</v>
+      </c>
+      <c r="N28">
+        <v>0.43</v>
+      </c>
+      <c r="O28">
+        <f>M28-N28</f>
+        <v>-2.9999999999999971E-2</v>
+      </c>
+      <c r="P28">
+        <v>1367</v>
+      </c>
+      <c r="Q28">
+        <v>2.4</v>
+      </c>
+      <c r="R28">
+        <v>2.37</v>
+      </c>
+      <c r="S28">
+        <f>Q28-R28</f>
+        <v>2.9999999999999805E-2</v>
+      </c>
+      <c r="T28">
+        <v>940</v>
+      </c>
+      <c r="U28">
+        <v>1.55</v>
+      </c>
+      <c r="V28">
+        <v>1.63</v>
+      </c>
+      <c r="W28">
+        <f>U28-V28</f>
+        <v>-7.9999999999999849E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:23" x14ac:dyDescent="0.35">
       <c r="H29" s="8">
         <v>80.890960000000007</v>
       </c>
@@ -1482,8 +1716,47 @@
         <f>H29/I29</f>
         <v>30.070988847583646</v>
       </c>
-    </row>
-    <row r="30" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="L29">
+        <v>1007</v>
+      </c>
+      <c r="M29">
+        <v>1.75</v>
+      </c>
+      <c r="N29">
+        <v>1.75</v>
+      </c>
+      <c r="O29">
+        <f t="shared" ref="O29:O30" si="46">M29-N29</f>
+        <v>0</v>
+      </c>
+      <c r="P29">
+        <v>4312</v>
+      </c>
+      <c r="Q29">
+        <v>8.0500000000000007</v>
+      </c>
+      <c r="R29">
+        <v>7.49</v>
+      </c>
+      <c r="S29">
+        <f t="shared" ref="S29:S30" si="47">Q29-R29</f>
+        <v>0.5600000000000005</v>
+      </c>
+      <c r="T29">
+        <v>2516</v>
+      </c>
+      <c r="U29">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="V29">
+        <v>4.37</v>
+      </c>
+      <c r="W29">
+        <f>U29-V29</f>
+        <v>-0.21999999999999975</v>
+      </c>
+    </row>
+    <row r="30" spans="2:23" x14ac:dyDescent="0.35">
       <c r="I30">
         <v>2.5</v>
       </c>
@@ -1491,15 +1764,134 @@
         <f>(J28+J29)/2</f>
         <v>29.334110460748349</v>
       </c>
-    </row>
-    <row r="31" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="L30">
+        <v>1063</v>
+      </c>
+      <c r="M30">
+        <v>1.65</v>
+      </c>
+      <c r="N30">
+        <v>1.85</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="46"/>
+        <v>-0.20000000000000018</v>
+      </c>
+      <c r="P30">
+        <v>5679</v>
+      </c>
+      <c r="Q30">
+        <v>10.45</v>
+      </c>
+      <c r="R30">
+        <v>9.86</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="47"/>
+        <v>0.58999999999999986</v>
+      </c>
+    </row>
+    <row r="31" spans="2:23" x14ac:dyDescent="0.35">
       <c r="J31">
         <f>J30*I30</f>
         <v>73.335276151870872</v>
       </c>
     </row>
+    <row r="33" spans="12:23" x14ac:dyDescent="0.35">
+      <c r="L33">
+        <f>247/-0.03</f>
+        <v>-8233.3333333333339</v>
+      </c>
+      <c r="P33">
+        <f>P28/S28</f>
+        <v>45566.666666666963</v>
+      </c>
+      <c r="T33">
+        <f>T28/W28</f>
+        <v>-11750.000000000022</v>
+      </c>
+    </row>
+    <row r="34" spans="12:23" x14ac:dyDescent="0.35">
+      <c r="L34">
+        <f>1063/-0.2</f>
+        <v>-5315</v>
+      </c>
+      <c r="P34">
+        <f t="shared" ref="P34:P35" si="48">P29/S29</f>
+        <v>7699.9999999999927</v>
+      </c>
+      <c r="T34">
+        <f>T29/W29</f>
+        <v>-11436.363636363649</v>
+      </c>
+    </row>
+    <row r="35" spans="12:23" x14ac:dyDescent="0.35">
+      <c r="P35">
+        <f t="shared" si="48"/>
+        <v>9625.423728813561</v>
+      </c>
+    </row>
+    <row r="37" spans="12:23" x14ac:dyDescent="0.35">
+      <c r="L37">
+        <f>5679/1063</f>
+        <v>5.3424270931326436</v>
+      </c>
+      <c r="T37">
+        <f>P30/T29</f>
+        <v>2.257154213036566</v>
+      </c>
+    </row>
+    <row r="38" spans="12:23" x14ac:dyDescent="0.35">
+      <c r="L38">
+        <f>L30*L37</f>
+        <v>5679</v>
+      </c>
+      <c r="O38">
+        <f>O30*L37</f>
+        <v>-1.0684854186265296</v>
+      </c>
+      <c r="T38">
+        <f>T29*T37</f>
+        <v>5679</v>
+      </c>
+      <c r="W38">
+        <f>W29*T37</f>
+        <v>-0.49657392686804397</v>
+      </c>
+    </row>
+    <row r="44" spans="12:23" x14ac:dyDescent="0.35">
+      <c r="L44">
+        <v>65.77</v>
+      </c>
+      <c r="N44">
+        <v>80.89</v>
+      </c>
+      <c r="P44">
+        <v>74</v>
+      </c>
+      <c r="R44">
+        <v>77.150000000000006</v>
+      </c>
+    </row>
+    <row r="45" spans="12:23" x14ac:dyDescent="0.35">
+      <c r="L45">
+        <f>O38</f>
+        <v>-1.0684854186265296</v>
+      </c>
+      <c r="N45">
+        <f>S30</f>
+        <v>0.58999999999999986</v>
+      </c>
+      <c r="P45">
+        <f>W38</f>
+        <v>-0.49657392686804397</v>
+      </c>
+      <c r="R45">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="V4:V17">
+  <conditionalFormatting sqref="V4:V19">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Added Measurements and updated TMC controller
</commit_message>
<xml_diff>
--- a/Measurements.xlsx
+++ b/Measurements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Perfusion_System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E81EA3-F260-41A5-A802-1D5945363D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF34C13-7E26-4019-B772-C462A291048B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Raw_High</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>Expected Vol for Perfusion</t>
+  </si>
+  <si>
+    <t>Short Duration, less accuracy</t>
   </si>
 </sst>
 </file>
@@ -189,9 +192,6 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -212,6 +212,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.000"/>
@@ -274,8 +277,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5A39537A-AD85-40E4-8132-CD746B4A4B1E}" name="Table1" displayName="Table1" ref="B3:L19" totalsRowShown="0">
-  <autoFilter ref="B3:L19" xr:uid="{5A39537A-AD85-40E4-8132-CD746B4A4B1E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5A39537A-AD85-40E4-8132-CD746B4A4B1E}" name="Table1" displayName="Table1" ref="B3:L21" totalsRowShown="0">
+  <autoFilter ref="B3:L21" xr:uid="{5A39537A-AD85-40E4-8132-CD746B4A4B1E}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{7F49C8BC-1009-4421-9279-20BA630C3F5B}" name="Index"/>
     <tableColumn id="2" xr3:uid="{5E47D918-C96A-47BF-882D-1F6F0C3B3A06}" name="Raw_High"/>
@@ -309,7 +312,7 @@
     <tableColumn id="3" xr3:uid="{CE281EF5-AD90-4E03-8914-DD9A9D900FAD}" name="Volume by Weight" dataDxfId="3">
       <calculatedColumnFormula>(F4-E4)/0.9982</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{9AD10D29-13FB-4A61-B0DA-D4754470DC60}" name="Expected Vol for Perfusion" dataDxfId="0">
+    <tableColumn id="5" xr3:uid="{9AD10D29-13FB-4A61-B0DA-D4754470DC60}" name="Expected Vol for Perfusion" dataDxfId="2">
       <calculatedColumnFormula>K4*P4</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -321,8 +324,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B419AA0D-6755-4C9D-BD52-00C6A845A2F0}" name="Table3" displayName="Table3" ref="U3:V11" totalsRowShown="0">
   <autoFilter ref="U3:V11" xr:uid="{B419AA0D-6755-4C9D-BD52-00C6A845A2F0}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{63D487F6-0EFF-42C3-90F0-E4DF35C983DE}" name="Flow-Rate" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{805730DE-BF4F-464F-9520-598D1BFA9242}" name="Accuracy" dataDxfId="1" dataCellStyle="Percent">
+    <tableColumn id="1" xr3:uid="{63D487F6-0EFF-42C3-90F0-E4DF35C983DE}" name="Flow-Rate" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{805730DE-BF4F-464F-9520-598D1BFA9242}" name="Accuracy" dataDxfId="0" dataCellStyle="Percent">
       <calculatedColumnFormula>(1-ABS(U4-K4)/K4)*100%</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -595,8 +598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:W45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="R44" sqref="R44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1643,6 +1646,129 @@
         <v>0.95007949125596203</v>
       </c>
     </row>
+    <row r="20" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="B20">
+        <v>17</v>
+      </c>
+      <c r="C20">
+        <v>286</v>
+      </c>
+      <c r="D20">
+        <v>159</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20" s="6">
+        <v>45882.546527777777</v>
+      </c>
+      <c r="H20" s="6">
+        <v>45883.46597222222</v>
+      </c>
+      <c r="I20">
+        <v>7.45</v>
+      </c>
+      <c r="J20">
+        <v>5.2</v>
+      </c>
+      <c r="K20">
+        <v>2.5</v>
+      </c>
+      <c r="O20" s="3">
+        <f t="shared" ref="O20" si="46">H20-G20</f>
+        <v>0.91944444444379769</v>
+      </c>
+      <c r="P20" s="4">
+        <f t="shared" ref="P20" si="47">O20</f>
+        <v>0.91944444444379769</v>
+      </c>
+      <c r="Q20" s="5">
+        <f t="shared" ref="Q20" si="48">I20-J20</f>
+        <v>2.25</v>
+      </c>
+      <c r="R20" s="1">
+        <f t="shared" ref="R20" si="49">(F20-E20)/0.9982</f>
+        <v>0</v>
+      </c>
+      <c r="S20" s="5">
+        <f>K20*P20</f>
+        <v>2.2986111111094942</v>
+      </c>
+      <c r="U20" s="1">
+        <f>Q20*1440/1324</f>
+        <v>2.4471299093655587</v>
+      </c>
+      <c r="V20" s="7">
+        <f t="shared" ref="V20" si="50">(1-ABS(U20-K20)/K20)*100%</f>
+        <v>0.97885196374622352</v>
+      </c>
+    </row>
+    <row r="21" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="B21">
+        <v>18</v>
+      </c>
+      <c r="C21">
+        <v>286</v>
+      </c>
+      <c r="D21">
+        <v>159</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21" s="6">
+        <v>45883.520833333336</v>
+      </c>
+      <c r="H21" s="6">
+        <v>45883.713194444441</v>
+      </c>
+      <c r="I21">
+        <v>5</v>
+      </c>
+      <c r="J21">
+        <v>4.55</v>
+      </c>
+      <c r="K21">
+        <v>2.5</v>
+      </c>
+      <c r="L21" t="s">
+        <v>20</v>
+      </c>
+      <c r="O21" s="3">
+        <f t="shared" ref="O21" si="51">H21-G21</f>
+        <v>0.19236111110512866</v>
+      </c>
+      <c r="P21" s="4">
+        <f t="shared" ref="P21" si="52">O21</f>
+        <v>0.19236111110512866</v>
+      </c>
+      <c r="Q21" s="5">
+        <f t="shared" ref="Q21" si="53">I21-J21</f>
+        <v>0.45000000000000018</v>
+      </c>
+      <c r="R21" s="1">
+        <f t="shared" ref="R21" si="54">(F21-E21)/0.9982</f>
+        <v>0</v>
+      </c>
+      <c r="S21" s="5">
+        <f>K21*P21</f>
+        <v>0.48090277776282164</v>
+      </c>
+      <c r="U21" s="1">
+        <f>Q21*1440/277</f>
+        <v>2.339350180505416</v>
+      </c>
+      <c r="V21" s="7">
+        <f t="shared" ref="V21" si="55">(1-ABS(U21-K21)/K21)*100%</f>
+        <v>0.93574007220216637</v>
+      </c>
+    </row>
     <row r="27" spans="2:23" x14ac:dyDescent="0.35">
       <c r="L27">
         <v>65.77</v>
@@ -1726,7 +1852,7 @@
         <v>1.75</v>
       </c>
       <c r="O29">
-        <f t="shared" ref="O29:O30" si="46">M29-N29</f>
+        <f t="shared" ref="O29:O30" si="56">M29-N29</f>
         <v>0</v>
       </c>
       <c r="P29">
@@ -1739,7 +1865,7 @@
         <v>7.49</v>
       </c>
       <c r="S29">
-        <f t="shared" ref="S29:S30" si="47">Q29-R29</f>
+        <f t="shared" ref="S29:S30" si="57">Q29-R29</f>
         <v>0.5600000000000005</v>
       </c>
       <c r="T29">
@@ -1774,7 +1900,7 @@
         <v>1.85</v>
       </c>
       <c r="O30">
-        <f t="shared" si="46"/>
+        <f t="shared" si="56"/>
         <v>-0.20000000000000018</v>
       </c>
       <c r="P30">
@@ -1787,7 +1913,7 @@
         <v>9.86</v>
       </c>
       <c r="S30">
-        <f t="shared" si="47"/>
+        <f t="shared" si="57"/>
         <v>0.58999999999999986</v>
       </c>
     </row>
@@ -1817,7 +1943,7 @@
         <v>-5315</v>
       </c>
       <c r="P34">
-        <f t="shared" ref="P34:P35" si="48">P29/S29</f>
+        <f t="shared" ref="P34:P35" si="58">P29/S29</f>
         <v>7699.9999999999927</v>
       </c>
       <c r="T34">
@@ -1827,7 +1953,7 @@
     </row>
     <row r="35" spans="12:23" x14ac:dyDescent="0.35">
       <c r="P35">
-        <f t="shared" si="48"/>
+        <f t="shared" si="58"/>
         <v>9625.423728813561</v>
       </c>
     </row>
@@ -1891,7 +2017,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="V4:V19">
+  <conditionalFormatting sqref="V4:V21">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
New pressure sensor added to the controller
</commit_message>
<xml_diff>
--- a/Measurements.xlsx
+++ b/Measurements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Perfusion_System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF34C13-7E26-4019-B772-C462A291048B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A639C5BA-F6EA-4E10-BD32-0D02AF0CB56C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -277,8 +277,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5A39537A-AD85-40E4-8132-CD746B4A4B1E}" name="Table1" displayName="Table1" ref="B3:L21" totalsRowShown="0">
-  <autoFilter ref="B3:L21" xr:uid="{5A39537A-AD85-40E4-8132-CD746B4A4B1E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5A39537A-AD85-40E4-8132-CD746B4A4B1E}" name="Table1" displayName="Table1" ref="B3:L22" totalsRowShown="0">
+  <autoFilter ref="B3:L22" xr:uid="{5A39537A-AD85-40E4-8132-CD746B4A4B1E}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{7F49C8BC-1009-4421-9279-20BA630C3F5B}" name="Index"/>
     <tableColumn id="2" xr3:uid="{5E47D918-C96A-47BF-882D-1F6F0C3B3A06}" name="Raw_High"/>
@@ -596,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:W45"/>
+  <dimension ref="B3:V45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P52" sqref="P52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1466,7 +1466,7 @@
         <v>0.94009508716323309</v>
       </c>
     </row>
-    <row r="17" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B17">
         <v>14</v>
       </c>
@@ -1526,7 +1526,7 @@
         <v>0.92467532467532454</v>
       </c>
     </row>
-    <row r="18" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B18">
         <v>15</v>
       </c>
@@ -1586,7 +1586,7 @@
         <v>0.94978723404255361</v>
       </c>
     </row>
-    <row r="19" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B19">
         <v>16</v>
       </c>
@@ -1646,7 +1646,7 @@
         <v>0.95007949125596203</v>
       </c>
     </row>
-    <row r="20" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B20">
         <v>17</v>
       </c>
@@ -1706,7 +1706,7 @@
         <v>0.97885196374622352</v>
       </c>
     </row>
-    <row r="21" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B21">
         <v>18</v>
       </c>
@@ -1769,255 +1769,315 @@
         <v>0.93574007220216637</v>
       </c>
     </row>
-    <row r="27" spans="2:23" x14ac:dyDescent="0.35">
-      <c r="L27">
+    <row r="22" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="B22">
+        <v>19</v>
+      </c>
+      <c r="C22">
+        <v>286</v>
+      </c>
+      <c r="D22">
+        <v>159</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22" s="6">
+        <v>45887.504166666666</v>
+      </c>
+      <c r="H22" s="6">
+        <v>45888.709722222222</v>
+      </c>
+      <c r="I22">
+        <v>11.9</v>
+      </c>
+      <c r="J22">
+        <v>9</v>
+      </c>
+      <c r="K22">
+        <v>2.5</v>
+      </c>
+      <c r="O22" s="3">
+        <f t="shared" ref="O22" si="56">H22-G22</f>
+        <v>1.2055555555562023</v>
+      </c>
+      <c r="P22" s="4">
+        <f t="shared" ref="P22" si="57">O22</f>
+        <v>1.2055555555562023</v>
+      </c>
+      <c r="Q22" s="5">
+        <f t="shared" ref="Q22" si="58">I22-J22</f>
+        <v>2.9000000000000004</v>
+      </c>
+      <c r="R22" s="1">
+        <f t="shared" ref="R22" si="59">(F22-E22)/0.9982</f>
+        <v>0</v>
+      </c>
+      <c r="S22" s="5">
+        <f>K22*P22</f>
+        <v>3.0138888888905058</v>
+      </c>
+      <c r="U22" s="1">
+        <f>Q22*1440/1736</f>
+        <v>2.4055299539170512</v>
+      </c>
+      <c r="V22" s="7">
+        <f t="shared" ref="V22" si="60">(1-ABS(U22-K22)/K22)*100%</f>
+        <v>0.96221198156682042</v>
+      </c>
+    </row>
+    <row r="27" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="I27">
         <v>65.77</v>
       </c>
-      <c r="P27">
+      <c r="M27">
         <v>80.89</v>
       </c>
-      <c r="T27">
+      <c r="Q27">
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="2:23" x14ac:dyDescent="0.35">
-      <c r="H28" s="8">
+    <row r="28" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="E28" s="8">
         <v>65.773633770000004</v>
       </c>
+      <c r="F28">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G28">
+        <f>E28/F28</f>
+        <v>28.597232073913048</v>
+      </c>
       <c r="I28">
-        <v>2.2999999999999998</v>
+        <v>247</v>
       </c>
       <c r="J28">
-        <f>H28/I28</f>
-        <v>28.597232073913048</v>
+        <v>0.4</v>
+      </c>
+      <c r="K28">
+        <v>0.43</v>
       </c>
       <c r="L28">
-        <v>247</v>
+        <f>J28-K28</f>
+        <v>-2.9999999999999971E-2</v>
       </c>
       <c r="M28">
-        <v>0.4</v>
+        <v>1367</v>
       </c>
       <c r="N28">
-        <v>0.43</v>
+        <v>2.4</v>
       </c>
       <c r="O28">
-        <f>M28-N28</f>
-        <v>-2.9999999999999971E-2</v>
+        <v>2.37</v>
       </c>
       <c r="P28">
-        <v>1367</v>
+        <f>N28-O28</f>
+        <v>2.9999999999999805E-2</v>
       </c>
       <c r="Q28">
-        <v>2.4</v>
+        <v>940</v>
       </c>
       <c r="R28">
-        <v>2.37</v>
+        <v>1.55</v>
       </c>
       <c r="S28">
-        <f>Q28-R28</f>
-        <v>2.9999999999999805E-2</v>
+        <v>1.63</v>
       </c>
       <c r="T28">
-        <v>940</v>
-      </c>
-      <c r="U28">
-        <v>1.55</v>
-      </c>
-      <c r="V28">
-        <v>1.63</v>
-      </c>
-      <c r="W28">
-        <f>U28-V28</f>
+        <f>R28-S28</f>
         <v>-7.9999999999999849E-2</v>
       </c>
     </row>
-    <row r="29" spans="2:23" x14ac:dyDescent="0.35">
-      <c r="H29" s="8">
+    <row r="29" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="E29" s="8">
         <v>80.890960000000007</v>
       </c>
+      <c r="F29">
+        <v>2.69</v>
+      </c>
+      <c r="G29">
+        <f>E29/F29</f>
+        <v>30.070988847583646</v>
+      </c>
       <c r="I29">
-        <v>2.69</v>
+        <v>1007</v>
       </c>
       <c r="J29">
-        <f>H29/I29</f>
-        <v>30.070988847583646</v>
+        <v>1.75</v>
+      </c>
+      <c r="K29">
+        <v>1.75</v>
       </c>
       <c r="L29">
-        <v>1007</v>
+        <f t="shared" ref="L29:L30" si="61">J29-K29</f>
+        <v>0</v>
       </c>
       <c r="M29">
-        <v>1.75</v>
+        <v>4312</v>
       </c>
       <c r="N29">
-        <v>1.75</v>
+        <v>8.0500000000000007</v>
       </c>
       <c r="O29">
-        <f t="shared" ref="O29:O30" si="56">M29-N29</f>
-        <v>0</v>
+        <v>7.49</v>
       </c>
       <c r="P29">
-        <v>4312</v>
+        <f t="shared" ref="P29:P30" si="62">N29-O29</f>
+        <v>0.5600000000000005</v>
       </c>
       <c r="Q29">
-        <v>8.0500000000000007</v>
+        <v>2516</v>
       </c>
       <c r="R29">
-        <v>7.49</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="S29">
-        <f t="shared" ref="S29:S30" si="57">Q29-R29</f>
-        <v>0.5600000000000005</v>
+        <v>4.37</v>
       </c>
       <c r="T29">
-        <v>2516</v>
-      </c>
-      <c r="U29">
-        <v>4.1500000000000004</v>
-      </c>
-      <c r="V29">
-        <v>4.37</v>
-      </c>
-      <c r="W29">
-        <f>U29-V29</f>
+        <f>R29-S29</f>
         <v>-0.21999999999999975</v>
       </c>
     </row>
-    <row r="30" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="F30">
+        <v>2.5</v>
+      </c>
+      <c r="G30">
+        <f>(G28+G29)/2</f>
+        <v>29.334110460748349</v>
+      </c>
       <c r="I30">
-        <v>2.5</v>
+        <v>1063</v>
       </c>
       <c r="J30">
-        <f>(J28+J29)/2</f>
-        <v>29.334110460748349</v>
+        <v>1.65</v>
+      </c>
+      <c r="K30">
+        <v>1.85</v>
       </c>
       <c r="L30">
-        <v>1063</v>
+        <f t="shared" si="61"/>
+        <v>-0.20000000000000018</v>
       </c>
       <c r="M30">
-        <v>1.65</v>
+        <v>5679</v>
       </c>
       <c r="N30">
-        <v>1.85</v>
+        <v>10.45</v>
       </c>
       <c r="O30">
-        <f t="shared" si="56"/>
-        <v>-0.20000000000000018</v>
+        <v>9.86</v>
       </c>
       <c r="P30">
-        <v>5679</v>
-      </c>
-      <c r="Q30">
-        <v>10.45</v>
-      </c>
-      <c r="R30">
-        <v>9.86</v>
-      </c>
-      <c r="S30">
-        <f t="shared" si="57"/>
+        <f t="shared" si="62"/>
         <v>0.58999999999999986</v>
       </c>
     </row>
-    <row r="31" spans="2:23" x14ac:dyDescent="0.35">
-      <c r="J31">
-        <f>J30*I30</f>
+    <row r="31" spans="2:22" x14ac:dyDescent="0.35">
+      <c r="G31">
+        <f>G30*F30</f>
         <v>73.335276151870872</v>
       </c>
     </row>
-    <row r="33" spans="12:23" x14ac:dyDescent="0.35">
-      <c r="L33">
+    <row r="33" spans="9:20" x14ac:dyDescent="0.35">
+      <c r="I33">
         <f>247/-0.03</f>
         <v>-8233.3333333333339</v>
       </c>
-      <c r="P33">
-        <f>P28/S28</f>
+      <c r="M33">
+        <f>M28/P28</f>
         <v>45566.666666666963</v>
       </c>
-      <c r="T33">
-        <f>T28/W28</f>
+      <c r="Q33">
+        <f>Q28/T28</f>
         <v>-11750.000000000022</v>
       </c>
     </row>
-    <row r="34" spans="12:23" x14ac:dyDescent="0.35">
-      <c r="L34">
+    <row r="34" spans="9:20" x14ac:dyDescent="0.35">
+      <c r="I34">
         <f>1063/-0.2</f>
         <v>-5315</v>
       </c>
-      <c r="P34">
-        <f t="shared" ref="P34:P35" si="58">P29/S29</f>
+      <c r="M34">
+        <f t="shared" ref="M34:M35" si="63">M29/P29</f>
         <v>7699.9999999999927</v>
       </c>
-      <c r="T34">
-        <f>T29/W29</f>
+      <c r="Q34">
+        <f>Q29/T29</f>
         <v>-11436.363636363649</v>
       </c>
     </row>
-    <row r="35" spans="12:23" x14ac:dyDescent="0.35">
-      <c r="P35">
-        <f t="shared" si="58"/>
+    <row r="35" spans="9:20" x14ac:dyDescent="0.35">
+      <c r="M35">
+        <f t="shared" si="63"/>
         <v>9625.423728813561</v>
       </c>
     </row>
-    <row r="37" spans="12:23" x14ac:dyDescent="0.35">
-      <c r="L37">
+    <row r="37" spans="9:20" x14ac:dyDescent="0.35">
+      <c r="I37">
         <f>5679/1063</f>
         <v>5.3424270931326436</v>
       </c>
-      <c r="T37">
-        <f>P30/T29</f>
+      <c r="Q37">
+        <f>M30/Q29</f>
         <v>2.257154213036566</v>
       </c>
     </row>
-    <row r="38" spans="12:23" x14ac:dyDescent="0.35">
+    <row r="38" spans="9:20" x14ac:dyDescent="0.35">
+      <c r="I38">
+        <f>I30*I37</f>
+        <v>5679</v>
+      </c>
       <c r="L38">
-        <f>L30*L37</f>
+        <f>L30*I37</f>
+        <v>-1.0684854186265296</v>
+      </c>
+      <c r="Q38">
+        <f>Q29*Q37</f>
         <v>5679</v>
       </c>
-      <c r="O38">
-        <f>O30*L37</f>
+      <c r="T38">
+        <f>T29*Q37</f>
+        <v>-0.49657392686804397</v>
+      </c>
+    </row>
+    <row r="44" spans="9:20" x14ac:dyDescent="0.35">
+      <c r="I44">
+        <v>65.77</v>
+      </c>
+      <c r="K44">
+        <v>80.89</v>
+      </c>
+      <c r="M44">
+        <v>74</v>
+      </c>
+      <c r="O44">
+        <v>77.150000000000006</v>
+      </c>
+    </row>
+    <row r="45" spans="9:20" x14ac:dyDescent="0.35">
+      <c r="I45">
+        <f>L38</f>
         <v>-1.0684854186265296</v>
       </c>
-      <c r="T38">
-        <f>T29*T37</f>
-        <v>5679</v>
-      </c>
-      <c r="W38">
-        <f>W29*T37</f>
+      <c r="K45">
+        <f>P30</f>
+        <v>0.58999999999999986</v>
+      </c>
+      <c r="M45">
+        <f>T38</f>
         <v>-0.49657392686804397</v>
       </c>
-    </row>
-    <row r="44" spans="12:23" x14ac:dyDescent="0.35">
-      <c r="L44">
-        <v>65.77</v>
-      </c>
-      <c r="N44">
-        <v>80.89</v>
-      </c>
-      <c r="P44">
-        <v>74</v>
-      </c>
-      <c r="R44">
-        <v>77.150000000000006</v>
-      </c>
-    </row>
-    <row r="45" spans="12:23" x14ac:dyDescent="0.35">
-      <c r="L45">
-        <f>O38</f>
-        <v>-1.0684854186265296</v>
-      </c>
-      <c r="N45">
-        <f>S30</f>
-        <v>0.58999999999999986</v>
-      </c>
-      <c r="P45">
-        <f>W38</f>
-        <v>-0.49657392686804397</v>
-      </c>
-      <c r="R45">
+      <c r="O45">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="V4:V21">
+  <conditionalFormatting sqref="V4:V22">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Add a measurement and changed speed in TMC.cpp
</commit_message>
<xml_diff>
--- a/Measurements.xlsx
+++ b/Measurements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Perfusion_System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A639C5BA-F6EA-4E10-BD32-0D02AF0CB56C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FECC7799-2B1C-4685-BD35-837A5415C9E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="38560" windowHeight="21160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -277,8 +277,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5A39537A-AD85-40E4-8132-CD746B4A4B1E}" name="Table1" displayName="Table1" ref="B3:L22" totalsRowShown="0">
-  <autoFilter ref="B3:L22" xr:uid="{5A39537A-AD85-40E4-8132-CD746B4A4B1E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5A39537A-AD85-40E4-8132-CD746B4A4B1E}" name="Table1" displayName="Table1" ref="B3:L26" totalsRowShown="0">
+  <autoFilter ref="B3:L26" xr:uid="{5A39537A-AD85-40E4-8132-CD746B4A4B1E}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{7F49C8BC-1009-4421-9279-20BA630C3F5B}" name="Index"/>
     <tableColumn id="2" xr3:uid="{5E47D918-C96A-47BF-882D-1F6F0C3B3A06}" name="Raw_High"/>
@@ -596,34 +596,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:V45"/>
+  <dimension ref="B3:AO26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P52" sqref="P52"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.36328125" customWidth="1"/>
-    <col min="3" max="4" width="12.08984375" customWidth="1"/>
-    <col min="5" max="5" width="16.7265625" customWidth="1"/>
-    <col min="6" max="6" width="15.1796875" customWidth="1"/>
-    <col min="7" max="7" width="21.7265625" customWidth="1"/>
-    <col min="8" max="8" width="22.08984375" customWidth="1"/>
-    <col min="9" max="9" width="18.90625" customWidth="1"/>
-    <col min="10" max="10" width="18.36328125" customWidth="1"/>
-    <col min="11" max="11" width="20.6328125" customWidth="1"/>
-    <col min="12" max="12" width="23.453125" customWidth="1"/>
-    <col min="15" max="15" width="12.453125" customWidth="1"/>
-    <col min="16" max="16" width="16.26953125" customWidth="1"/>
-    <col min="17" max="17" width="18.54296875" customWidth="1"/>
-    <col min="18" max="18" width="19.7265625" customWidth="1"/>
-    <col min="19" max="19" width="25.36328125" customWidth="1"/>
-    <col min="21" max="21" width="11.54296875" customWidth="1"/>
-    <col min="22" max="22" width="10.6328125" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" customWidth="1"/>
+    <col min="8" max="8" width="22.140625" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" customWidth="1"/>
+    <col min="11" max="11" width="20.5703125" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" customWidth="1"/>
+    <col min="16" max="16" width="16.28515625" customWidth="1"/>
+    <col min="17" max="17" width="18.5703125" customWidth="1"/>
+    <col min="18" max="18" width="19.7109375" customWidth="1"/>
+    <col min="19" max="19" width="25.42578125" customWidth="1"/>
+    <col min="21" max="21" width="11.5703125" customWidth="1"/>
+    <col min="22" max="22" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -678,8 +678,17 @@
       <c r="V3" t="s">
         <v>18</v>
       </c>
+      <c r="AD3">
+        <v>65.77</v>
+      </c>
+      <c r="AH3">
+        <v>80.89</v>
+      </c>
+      <c r="AL3">
+        <v>74</v>
+      </c>
     </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
@@ -742,8 +751,57 @@
         <f>(1-ABS(U4-K4)/K4)*100%</f>
         <v>0.83920529801324473</v>
       </c>
+      <c r="Z4" s="8">
+        <v>65.773633770000004</v>
+      </c>
+      <c r="AA4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AB4">
+        <f>Z4/AA4</f>
+        <v>28.597232073913048</v>
+      </c>
+      <c r="AD4">
+        <v>247</v>
+      </c>
+      <c r="AE4">
+        <v>0.4</v>
+      </c>
+      <c r="AF4">
+        <v>0.43</v>
+      </c>
+      <c r="AG4">
+        <f>AE4-AF4</f>
+        <v>-2.9999999999999971E-2</v>
+      </c>
+      <c r="AH4">
+        <v>1367</v>
+      </c>
+      <c r="AI4">
+        <v>2.4</v>
+      </c>
+      <c r="AJ4">
+        <v>2.37</v>
+      </c>
+      <c r="AK4">
+        <f>AI4-AJ4</f>
+        <v>2.9999999999999805E-2</v>
+      </c>
+      <c r="AL4">
+        <v>940</v>
+      </c>
+      <c r="AM4">
+        <v>1.55</v>
+      </c>
+      <c r="AN4">
+        <v>1.63</v>
+      </c>
+      <c r="AO4">
+        <f>AM4-AN4</f>
+        <v>-7.9999999999999849E-2</v>
+      </c>
     </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>2</v>
       </c>
@@ -773,6 +831,9 @@
       </c>
       <c r="K5">
         <v>2.5</v>
+      </c>
+      <c r="L5">
+        <v>65.77</v>
       </c>
       <c r="O5" s="3">
         <f t="shared" si="0"/>
@@ -802,8 +863,57 @@
         <f t="shared" ref="V5:V11" si="5">(1-ABS(U5-K5)/K5)*100%</f>
         <v>0.93279352226720724</v>
       </c>
+      <c r="Z5" s="8">
+        <v>80.890960000000007</v>
+      </c>
+      <c r="AA5">
+        <v>2.69</v>
+      </c>
+      <c r="AB5">
+        <f>Z5/AA5</f>
+        <v>30.070988847583646</v>
+      </c>
+      <c r="AD5">
+        <v>1007</v>
+      </c>
+      <c r="AE5">
+        <v>1.75</v>
+      </c>
+      <c r="AF5">
+        <v>1.75</v>
+      </c>
+      <c r="AG5">
+        <f t="shared" ref="AG5:AG6" si="6">AE5-AF5</f>
+        <v>0</v>
+      </c>
+      <c r="AH5">
+        <v>4312</v>
+      </c>
+      <c r="AI5">
+        <v>8.0500000000000007</v>
+      </c>
+      <c r="AJ5">
+        <v>7.49</v>
+      </c>
+      <c r="AK5">
+        <f t="shared" ref="AK5:AK6" si="7">AI5-AJ5</f>
+        <v>0.5600000000000005</v>
+      </c>
+      <c r="AL5">
+        <v>2516</v>
+      </c>
+      <c r="AM5">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="AN5">
+        <v>4.37</v>
+      </c>
+      <c r="AO5">
+        <f>AM5-AN5</f>
+        <v>-0.21999999999999975</v>
+      </c>
     </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>3</v>
       </c>
@@ -862,8 +972,41 @@
         <f t="shared" si="5"/>
         <v>0.90342205323193936</v>
       </c>
+      <c r="AA6">
+        <v>2.5</v>
+      </c>
+      <c r="AB6">
+        <f>(AB4+AB5)/2</f>
+        <v>29.334110460748349</v>
+      </c>
+      <c r="AD6">
+        <v>1063</v>
+      </c>
+      <c r="AE6">
+        <v>1.65</v>
+      </c>
+      <c r="AF6">
+        <v>1.85</v>
+      </c>
+      <c r="AG6">
+        <f t="shared" si="6"/>
+        <v>-0.20000000000000018</v>
+      </c>
+      <c r="AH6">
+        <v>5679</v>
+      </c>
+      <c r="AI6">
+        <v>10.45</v>
+      </c>
+      <c r="AJ6">
+        <v>9.86</v>
+      </c>
+      <c r="AK6">
+        <f t="shared" si="7"/>
+        <v>0.58999999999999986</v>
+      </c>
     </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>4</v>
       </c>
@@ -922,8 +1065,12 @@
         <f t="shared" si="5"/>
         <v>0.84705882352941175</v>
       </c>
+      <c r="AB7">
+        <f>AB6*AA6</f>
+        <v>73.335276151870872</v>
+      </c>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>5</v>
       </c>
@@ -986,7 +1133,7 @@
         <v>0.89704918032786907</v>
       </c>
     </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>6</v>
       </c>
@@ -1016,6 +1163,9 @@
       </c>
       <c r="K9">
         <v>25</v>
+      </c>
+      <c r="L9">
+        <v>80.89</v>
       </c>
       <c r="O9" s="3">
         <f t="shared" si="0"/>
@@ -1045,8 +1195,20 @@
         <f t="shared" si="5"/>
         <v>0.89563909774436101</v>
       </c>
+      <c r="AD9">
+        <f>247/-0.03</f>
+        <v>-8233.3333333333339</v>
+      </c>
+      <c r="AH9">
+        <f>AH4/AK4</f>
+        <v>45566.666666666963</v>
+      </c>
+      <c r="AL9">
+        <f>AL4/AO4</f>
+        <v>-11750.000000000022</v>
+      </c>
     </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>7</v>
       </c>
@@ -1105,8 +1267,20 @@
         <f t="shared" si="5"/>
         <v>0.8815533980582525</v>
       </c>
+      <c r="AD10">
+        <f>1063/-0.2</f>
+        <v>-5315</v>
+      </c>
+      <c r="AH10">
+        <f t="shared" ref="AH10:AH11" si="8">AH5/AK5</f>
+        <v>7699.9999999999927</v>
+      </c>
+      <c r="AL10">
+        <f>AL5/AO5</f>
+        <v>-11436.363636363649</v>
+      </c>
     </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>8</v>
       </c>
@@ -1165,8 +1339,12 @@
         <f t="shared" si="5"/>
         <v>0.99900695134061568</v>
       </c>
+      <c r="AH11">
+        <f t="shared" si="8"/>
+        <v>9625.423728813561</v>
+      </c>
     </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>9</v>
       </c>
@@ -1198,19 +1376,19 @@
         <v>25</v>
       </c>
       <c r="O12" s="3">
-        <f t="shared" ref="O12" si="6">H12-G12</f>
+        <f t="shared" ref="O12" si="9">H12-G12</f>
         <v>9.7916666665696539E-2</v>
       </c>
       <c r="P12" s="4">
-        <f t="shared" ref="P12" si="7">O12</f>
+        <f t="shared" ref="P12" si="10">O12</f>
         <v>9.7916666665696539E-2</v>
       </c>
       <c r="Q12" s="5">
-        <f t="shared" ref="Q12" si="8">I12-J12</f>
+        <f t="shared" ref="Q12" si="11">I12-J12</f>
         <v>2.4499999999999993</v>
       </c>
       <c r="R12" s="1">
-        <f t="shared" ref="R12" si="9">(F12-E12)/0.9982</f>
+        <f t="shared" ref="R12" si="12">(F12-E12)/0.9982</f>
         <v>0</v>
       </c>
       <c r="S12" s="5">
@@ -1222,11 +1400,11 @@
         <v>25.021276595744673</v>
       </c>
       <c r="V12" s="7">
-        <f t="shared" ref="V12" si="10">(1-ABS(U12-K12)/K12)*100%</f>
+        <f t="shared" ref="V12" si="13">(1-ABS(U12-K12)/K12)*100%</f>
         <v>0.99914893617021305</v>
       </c>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>10</v>
       </c>
@@ -1258,19 +1436,19 @@
         <v>25</v>
       </c>
       <c r="O13" s="3">
-        <f t="shared" ref="O13" si="11">H13-G13</f>
+        <f t="shared" ref="O13" si="14">H13-G13</f>
         <v>0.14513888888905058</v>
       </c>
       <c r="P13" s="4">
-        <f t="shared" ref="P13" si="12">O13</f>
+        <f t="shared" ref="P13" si="15">O13</f>
         <v>0.14513888888905058</v>
       </c>
       <c r="Q13" s="5">
-        <f t="shared" ref="Q13" si="13">I13-J13</f>
+        <f t="shared" ref="Q13" si="16">I13-J13</f>
         <v>3.5999999999999996</v>
       </c>
       <c r="R13" s="1">
-        <f t="shared" ref="R13" si="14">(F13-E13)/0.9982</f>
+        <f t="shared" ref="R13" si="17">(F13-E13)/0.9982</f>
         <v>0</v>
       </c>
       <c r="S13" s="5">
@@ -1282,11 +1460,19 @@
         <v>24.803827751196167</v>
       </c>
       <c r="V13" s="7">
-        <f t="shared" ref="V13" si="15">(1-ABS(U13-K13)/K13)*100%</f>
+        <f t="shared" ref="V13" si="18">(1-ABS(U13-K13)/K13)*100%</f>
         <v>0.99215311004784668</v>
       </c>
+      <c r="AD13">
+        <f>5679/1063</f>
+        <v>5.3424270931326436</v>
+      </c>
+      <c r="AL13">
+        <f>AH6/AL5</f>
+        <v>2.257154213036566</v>
+      </c>
     </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>11</v>
       </c>
@@ -1318,19 +1504,19 @@
         <v>5</v>
       </c>
       <c r="O14" s="3">
-        <f t="shared" ref="O14" si="16">H14-G14</f>
+        <f t="shared" ref="O14" si="19">H14-G14</f>
         <v>9.5138888893416151E-2</v>
       </c>
       <c r="P14" s="4">
-        <f t="shared" ref="P14" si="17">O14</f>
+        <f t="shared" ref="P14" si="20">O14</f>
         <v>9.5138888893416151E-2</v>
       </c>
       <c r="Q14" s="5">
-        <f t="shared" ref="Q14" si="18">I14-J14</f>
+        <f t="shared" ref="Q14" si="21">I14-J14</f>
         <v>0.51999999999999957</v>
       </c>
       <c r="R14" s="1">
-        <f t="shared" ref="R14" si="19">(F14-E14)/0.9982</f>
+        <f t="shared" ref="R14" si="22">(F14-E14)/0.9982</f>
         <v>0</v>
       </c>
       <c r="S14" s="5">
@@ -1342,11 +1528,27 @@
         <v>5.4656934306569296</v>
       </c>
       <c r="V14" s="7">
-        <f t="shared" ref="V14" si="20">(1-ABS(U14-K14)/K14)*100%</f>
+        <f t="shared" ref="V14" si="23">(1-ABS(U14-K14)/K14)*100%</f>
         <v>0.90686131386861413</v>
       </c>
+      <c r="AD14">
+        <f>AD6*AD13</f>
+        <v>5679</v>
+      </c>
+      <c r="AG14">
+        <f>AG6*AD13</f>
+        <v>-1.0684854186265296</v>
+      </c>
+      <c r="AL14">
+        <f>AL5*AL13</f>
+        <v>5679</v>
+      </c>
+      <c r="AO14">
+        <f>AO5*AL13</f>
+        <v>-0.49657392686804397</v>
+      </c>
     </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>12</v>
       </c>
@@ -1378,19 +1580,19 @@
         <v>2.5</v>
       </c>
       <c r="O15" s="3">
-        <f t="shared" ref="O15" si="21">H15-G15</f>
+        <f t="shared" ref="O15" si="24">H15-G15</f>
         <v>0.94930555555038154</v>
       </c>
       <c r="P15" s="4">
-        <f t="shared" ref="P15" si="22">O15</f>
+        <f t="shared" ref="P15" si="25">O15</f>
         <v>0.94930555555038154</v>
       </c>
       <c r="Q15" s="5">
-        <f t="shared" ref="Q15" si="23">I15-J15</f>
+        <f t="shared" ref="Q15" si="26">I15-J15</f>
         <v>2.3999999999999986</v>
       </c>
       <c r="R15" s="1">
-        <f t="shared" ref="R15" si="24">(F15-E15)/0.9982</f>
+        <f t="shared" ref="R15" si="27">(F15-E15)/0.9982</f>
         <v>0</v>
       </c>
       <c r="S15" s="5">
@@ -1402,11 +1604,11 @@
         <v>2.5281638624725664</v>
       </c>
       <c r="V15" s="7">
-        <f t="shared" ref="V15" si="25">(1-ABS(U15-K15)/K15)*100%</f>
+        <f t="shared" ref="V15" si="28">(1-ABS(U15-K15)/K15)*100%</f>
         <v>0.98873445501097346</v>
       </c>
     </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>13</v>
       </c>
@@ -1438,19 +1640,19 @@
         <v>2.5</v>
       </c>
       <c r="O16" s="3">
-        <f t="shared" ref="O16" si="26">H16-G16</f>
+        <f t="shared" ref="O16" si="29">H16-G16</f>
         <v>3.9437499999985448</v>
       </c>
       <c r="P16" s="4">
-        <f t="shared" ref="P16" si="27">O16</f>
+        <f t="shared" ref="P16" si="30">O16</f>
         <v>3.9437499999985448</v>
       </c>
       <c r="Q16" s="5">
-        <f t="shared" ref="Q16" si="28">I16-J16</f>
+        <f t="shared" ref="Q16" si="31">I16-J16</f>
         <v>10.45</v>
       </c>
       <c r="R16" s="1">
-        <f t="shared" ref="R16" si="29">(F16-E16)/0.9982</f>
+        <f t="shared" ref="R16" si="32">(F16-E16)/0.9982</f>
         <v>0</v>
       </c>
       <c r="S16" s="5">
@@ -1462,11 +1664,11 @@
         <v>2.6497622820919173</v>
       </c>
       <c r="V16" s="7">
-        <f t="shared" ref="V16" si="30">(1-ABS(U16-K16)/K16)*100%</f>
+        <f t="shared" ref="V16" si="33">(1-ABS(U16-K16)/K16)*100%</f>
         <v>0.94009508716323309</v>
       </c>
     </row>
-    <row r="17" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>14</v>
       </c>
@@ -1498,19 +1700,19 @@
         <v>2.5</v>
       </c>
       <c r="O17" s="3">
-        <f t="shared" ref="O17" si="31">H17-G17</f>
+        <f t="shared" ref="O17" si="34">H17-G17</f>
         <v>2.9944444444481633</v>
       </c>
       <c r="P17" s="4">
-        <f t="shared" ref="P17" si="32">O17</f>
+        <f t="shared" ref="P17" si="35">O17</f>
         <v>2.9944444444481633</v>
       </c>
       <c r="Q17" s="5">
-        <f t="shared" ref="Q17" si="33">I17-J17</f>
+        <f t="shared" ref="Q17" si="36">I17-J17</f>
         <v>8.0500000000000007</v>
       </c>
       <c r="R17" s="1">
-        <f t="shared" ref="R17" si="34">(F17-E17)/0.9982</f>
+        <f t="shared" ref="R17" si="37">(F17-E17)/0.9982</f>
         <v>0</v>
       </c>
       <c r="S17" s="5">
@@ -1522,11 +1724,11 @@
         <v>2.6883116883116887</v>
       </c>
       <c r="V17" s="7">
-        <f t="shared" ref="V17" si="35">(1-ABS(U17-K17)/K17)*100%</f>
+        <f t="shared" ref="V17" si="38">(1-ABS(U17-K17)/K17)*100%</f>
         <v>0.92467532467532454</v>
       </c>
     </row>
-    <row r="18" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>15</v>
       </c>
@@ -1557,20 +1759,23 @@
       <c r="K18">
         <v>2.5</v>
       </c>
+      <c r="L18">
+        <v>74</v>
+      </c>
       <c r="O18" s="3">
-        <f t="shared" ref="O18" si="36">H18-G18</f>
+        <f t="shared" ref="O18" si="39">H18-G18</f>
         <v>0.65277777777373558</v>
       </c>
       <c r="P18" s="4">
-        <f t="shared" ref="P18" si="37">O18</f>
+        <f t="shared" ref="P18" si="40">O18</f>
         <v>0.65277777777373558</v>
       </c>
       <c r="Q18" s="5">
-        <f t="shared" ref="Q18" si="38">I18-J18</f>
+        <f t="shared" ref="Q18" si="41">I18-J18</f>
         <v>1.5500000000000007</v>
       </c>
       <c r="R18" s="1">
-        <f t="shared" ref="R18" si="39">(F18-E18)/0.9982</f>
+        <f t="shared" ref="R18" si="42">(F18-E18)/0.9982</f>
         <v>0</v>
       </c>
       <c r="S18" s="5">
@@ -1582,11 +1787,11 @@
         <v>2.374468085106384</v>
       </c>
       <c r="V18" s="7">
-        <f t="shared" ref="V18" si="40">(1-ABS(U18-K18)/K18)*100%</f>
+        <f t="shared" ref="V18" si="43">(1-ABS(U18-K18)/K18)*100%</f>
         <v>0.94978723404255361</v>
       </c>
     </row>
-    <row r="19" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>16</v>
       </c>
@@ -1618,19 +1823,19 @@
         <v>2.5</v>
       </c>
       <c r="O19" s="3">
-        <f t="shared" ref="O19" si="41">H19-G19</f>
+        <f t="shared" ref="O19" si="44">H19-G19</f>
         <v>1.7472222222204437</v>
       </c>
       <c r="P19" s="4">
-        <f t="shared" ref="P19" si="42">O19</f>
+        <f t="shared" ref="P19" si="45">O19</f>
         <v>1.7472222222204437</v>
       </c>
       <c r="Q19" s="5">
-        <f t="shared" ref="Q19" si="43">I19-J19</f>
+        <f t="shared" ref="Q19" si="46">I19-J19</f>
         <v>4.1500000000000004</v>
       </c>
       <c r="R19" s="1">
-        <f t="shared" ref="R19" si="44">(F19-E19)/0.9982</f>
+        <f t="shared" ref="R19" si="47">(F19-E19)/0.9982</f>
         <v>0</v>
       </c>
       <c r="S19" s="5">
@@ -1642,11 +1847,11 @@
         <v>2.375198728139905</v>
       </c>
       <c r="V19" s="7">
-        <f t="shared" ref="V19" si="45">(1-ABS(U19-K19)/K19)*100%</f>
+        <f t="shared" ref="V19" si="48">(1-ABS(U19-K19)/K19)*100%</f>
         <v>0.95007949125596203</v>
       </c>
     </row>
-    <row r="20" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>17</v>
       </c>
@@ -1677,20 +1882,23 @@
       <c r="K20">
         <v>2.5</v>
       </c>
+      <c r="L20">
+        <v>77.150000000000006</v>
+      </c>
       <c r="O20" s="3">
-        <f t="shared" ref="O20" si="46">H20-G20</f>
+        <f t="shared" ref="O20" si="49">H20-G20</f>
         <v>0.91944444444379769</v>
       </c>
       <c r="P20" s="4">
-        <f t="shared" ref="P20" si="47">O20</f>
+        <f t="shared" ref="P20" si="50">O20</f>
         <v>0.91944444444379769</v>
       </c>
       <c r="Q20" s="5">
-        <f t="shared" ref="Q20" si="48">I20-J20</f>
+        <f t="shared" ref="Q20" si="51">I20-J20</f>
         <v>2.25</v>
       </c>
       <c r="R20" s="1">
-        <f t="shared" ref="R20" si="49">(F20-E20)/0.9982</f>
+        <f t="shared" ref="R20" si="52">(F20-E20)/0.9982</f>
         <v>0</v>
       </c>
       <c r="S20" s="5">
@@ -1702,11 +1910,23 @@
         <v>2.4471299093655587</v>
       </c>
       <c r="V20" s="7">
-        <f t="shared" ref="V20" si="50">(1-ABS(U20-K20)/K20)*100%</f>
+        <f t="shared" ref="V20" si="53">(1-ABS(U20-K20)/K20)*100%</f>
         <v>0.97885196374622352</v>
       </c>
+      <c r="AD20">
+        <v>65.77</v>
+      </c>
+      <c r="AF20">
+        <v>80.89</v>
+      </c>
+      <c r="AH20">
+        <v>74</v>
+      </c>
+      <c r="AJ20">
+        <v>77.150000000000006</v>
+      </c>
     </row>
-    <row r="21" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>18</v>
       </c>
@@ -1741,19 +1961,19 @@
         <v>20</v>
       </c>
       <c r="O21" s="3">
-        <f t="shared" ref="O21" si="51">H21-G21</f>
+        <f t="shared" ref="O21" si="54">H21-G21</f>
         <v>0.19236111110512866</v>
       </c>
       <c r="P21" s="4">
-        <f t="shared" ref="P21" si="52">O21</f>
+        <f t="shared" ref="P21" si="55">O21</f>
         <v>0.19236111110512866</v>
       </c>
       <c r="Q21" s="5">
-        <f t="shared" ref="Q21" si="53">I21-J21</f>
+        <f t="shared" ref="Q21" si="56">I21-J21</f>
         <v>0.45000000000000018</v>
       </c>
       <c r="R21" s="1">
-        <f t="shared" ref="R21" si="54">(F21-E21)/0.9982</f>
+        <f t="shared" ref="R21" si="57">(F21-E21)/0.9982</f>
         <v>0</v>
       </c>
       <c r="S21" s="5">
@@ -1765,11 +1985,26 @@
         <v>2.339350180505416</v>
       </c>
       <c r="V21" s="7">
-        <f t="shared" ref="V21" si="55">(1-ABS(U21-K21)/K21)*100%</f>
+        <f t="shared" ref="V21" si="58">(1-ABS(U21-K21)/K21)*100%</f>
         <v>0.93574007220216637</v>
       </c>
+      <c r="AD21">
+        <f>AG14</f>
+        <v>-1.0684854186265296</v>
+      </c>
+      <c r="AF21">
+        <f>AK6</f>
+        <v>0.58999999999999986</v>
+      </c>
+      <c r="AH21">
+        <f>AO14</f>
+        <v>-0.49657392686804397</v>
+      </c>
+      <c r="AJ21">
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="2:22" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:36" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>19</v>
       </c>
@@ -1801,19 +2036,19 @@
         <v>2.5</v>
       </c>
       <c r="O22" s="3">
-        <f t="shared" ref="O22" si="56">H22-G22</f>
+        <f t="shared" ref="O22" si="59">H22-G22</f>
         <v>1.2055555555562023</v>
       </c>
       <c r="P22" s="4">
-        <f t="shared" ref="P22" si="57">O22</f>
+        <f t="shared" ref="P22" si="60">O22</f>
         <v>1.2055555555562023</v>
       </c>
       <c r="Q22" s="5">
-        <f t="shared" ref="Q22" si="58">I22-J22</f>
+        <f t="shared" ref="Q22" si="61">I22-J22</f>
         <v>2.9000000000000004</v>
       </c>
       <c r="R22" s="1">
-        <f t="shared" ref="R22" si="59">(F22-E22)/0.9982</f>
+        <f t="shared" ref="R22" si="62">(F22-E22)/0.9982</f>
         <v>0</v>
       </c>
       <c r="S22" s="5">
@@ -1825,266 +2060,269 @@
         <v>2.4055299539170512</v>
       </c>
       <c r="V22" s="7">
-        <f t="shared" ref="V22" si="60">(1-ABS(U22-K22)/K22)*100%</f>
+        <f t="shared" ref="V22" si="63">(1-ABS(U22-K22)/K22)*100%</f>
         <v>0.96221198156682042</v>
       </c>
     </row>
-    <row r="27" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="I27">
-        <v>65.77</v>
-      </c>
-      <c r="M27">
-        <v>80.89</v>
-      </c>
-      <c r="Q27">
-        <v>74</v>
+    <row r="23" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>20</v>
+      </c>
+      <c r="C23">
+        <v>286</v>
+      </c>
+      <c r="D23">
+        <v>159</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23" s="6">
+        <v>45888.709722222222</v>
+      </c>
+      <c r="H23" s="6">
+        <v>45889.46597222222</v>
+      </c>
+      <c r="I23">
+        <v>9</v>
+      </c>
+      <c r="J23">
+        <v>7.2</v>
+      </c>
+      <c r="K23">
+        <v>2.5</v>
+      </c>
+      <c r="O23" s="3">
+        <f t="shared" ref="O23:O24" si="64">H23-G23</f>
+        <v>0.75624999999854481</v>
+      </c>
+      <c r="P23" s="4">
+        <f t="shared" ref="P23:P24" si="65">O23</f>
+        <v>0.75624999999854481</v>
+      </c>
+      <c r="Q23" s="5">
+        <f t="shared" ref="Q23:Q24" si="66">I23-J23</f>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="R23" s="1">
+        <f t="shared" ref="R23:R24" si="67">(F23-E23)/0.9982</f>
+        <v>0</v>
+      </c>
+      <c r="S23" s="5">
+        <f t="shared" ref="S23:S24" si="68">K23*P23</f>
+        <v>1.890624999996362</v>
+      </c>
+      <c r="U23" s="1">
+        <f>Q23*1440/1089</f>
+        <v>2.380165289256198</v>
+      </c>
+      <c r="V23" s="7">
+        <f t="shared" ref="V23:V24" si="69">(1-ABS(U23-K23)/K23)*100%</f>
+        <v>0.95206611570247923</v>
       </c>
     </row>
-    <row r="28" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="E28" s="8">
-        <v>65.773633770000004</v>
-      </c>
-      <c r="F28">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="G28">
-        <f>E28/F28</f>
-        <v>28.597232073913048</v>
-      </c>
-      <c r="I28">
-        <v>247</v>
-      </c>
-      <c r="J28">
-        <v>0.4</v>
-      </c>
-      <c r="K28">
-        <v>0.43</v>
-      </c>
-      <c r="L28">
-        <f>J28-K28</f>
-        <v>-2.9999999999999971E-2</v>
-      </c>
-      <c r="M28">
-        <v>1367</v>
-      </c>
-      <c r="N28">
-        <v>2.4</v>
-      </c>
-      <c r="O28">
-        <v>2.37</v>
-      </c>
-      <c r="P28">
-        <f>N28-O28</f>
-        <v>2.9999999999999805E-2</v>
-      </c>
-      <c r="Q28">
-        <v>940</v>
-      </c>
-      <c r="R28">
-        <v>1.55</v>
-      </c>
-      <c r="S28">
-        <v>1.63</v>
-      </c>
-      <c r="T28">
-        <f>R28-S28</f>
-        <v>-7.9999999999999849E-2</v>
+    <row r="24" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>21</v>
+      </c>
+      <c r="C24">
+        <v>286</v>
+      </c>
+      <c r="D24">
+        <v>159</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24" s="6">
+        <v>45887.504166666666</v>
+      </c>
+      <c r="H24" s="6">
+        <v>45889.606944444444</v>
+      </c>
+      <c r="I24">
+        <v>11.9</v>
+      </c>
+      <c r="J24">
+        <v>6.8</v>
+      </c>
+      <c r="K24">
+        <v>2.5</v>
+      </c>
+      <c r="O24" s="3">
+        <f t="shared" si="64"/>
+        <v>2.1027777777781012</v>
+      </c>
+      <c r="P24" s="4">
+        <f t="shared" si="65"/>
+        <v>2.1027777777781012</v>
+      </c>
+      <c r="Q24" s="5">
+        <f t="shared" si="66"/>
+        <v>5.1000000000000005</v>
+      </c>
+      <c r="R24" s="1">
+        <f t="shared" si="67"/>
+        <v>0</v>
+      </c>
+      <c r="S24" s="5">
+        <f t="shared" si="68"/>
+        <v>5.2569444444452529</v>
+      </c>
+      <c r="U24" s="1">
+        <f>Q24*1440/3028</f>
+        <v>2.4253632760898287</v>
+      </c>
+      <c r="V24" s="7">
+        <f t="shared" si="69"/>
+        <v>0.97014531043593144</v>
       </c>
     </row>
-    <row r="29" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="E29" s="8">
-        <v>80.890960000000007</v>
-      </c>
-      <c r="F29">
-        <v>2.69</v>
-      </c>
-      <c r="G29">
-        <f>E29/F29</f>
-        <v>30.070988847583646</v>
-      </c>
-      <c r="I29">
-        <v>1007</v>
-      </c>
-      <c r="J29">
-        <v>1.75</v>
-      </c>
-      <c r="K29">
-        <v>1.75</v>
-      </c>
-      <c r="L29">
-        <f t="shared" ref="L29:L30" si="61">J29-K29</f>
-        <v>0</v>
-      </c>
-      <c r="M29">
-        <v>4312</v>
-      </c>
-      <c r="N29">
-        <v>8.0500000000000007</v>
-      </c>
-      <c r="O29">
-        <v>7.49</v>
-      </c>
-      <c r="P29">
-        <f t="shared" ref="P29:P30" si="62">N29-O29</f>
-        <v>0.5600000000000005</v>
-      </c>
-      <c r="Q29">
-        <v>2516</v>
-      </c>
-      <c r="R29">
-        <v>4.1500000000000004</v>
-      </c>
-      <c r="S29">
-        <v>4.37</v>
-      </c>
-      <c r="T29">
-        <f>R29-S29</f>
-        <v>-0.21999999999999975</v>
+    <row r="25" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>22</v>
+      </c>
+      <c r="C25">
+        <v>286</v>
+      </c>
+      <c r="D25">
+        <v>159</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25" s="6">
+        <v>45889.631249999999</v>
+      </c>
+      <c r="H25" s="6">
+        <v>45890.431250000001</v>
+      </c>
+      <c r="I25">
+        <v>6.8</v>
+      </c>
+      <c r="J25">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="K25">
+        <v>2.5</v>
+      </c>
+      <c r="O25" s="3">
+        <f t="shared" ref="O25" si="70">H25-G25</f>
+        <v>0.80000000000291038</v>
+      </c>
+      <c r="P25" s="4">
+        <f t="shared" ref="P25" si="71">O25</f>
+        <v>0.80000000000291038</v>
+      </c>
+      <c r="Q25" s="5">
+        <f t="shared" ref="Q25" si="72">I25-J25</f>
+        <v>1.8999999999999995</v>
+      </c>
+      <c r="R25" s="1">
+        <f t="shared" ref="R25" si="73">(F25-E25)/0.9982</f>
+        <v>0</v>
+      </c>
+      <c r="S25" s="5">
+        <f t="shared" ref="S25" si="74">K25*P25</f>
+        <v>2.000000000007276</v>
+      </c>
+      <c r="U25" s="1">
+        <f>Q25*1440/1152</f>
+        <v>2.3749999999999991</v>
+      </c>
+      <c r="V25" s="7">
+        <f t="shared" ref="V25" si="75">(1-ABS(U25-K25)/K25)*100%</f>
+        <v>0.94999999999999962</v>
       </c>
     </row>
-    <row r="30" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="F30">
+    <row r="26" spans="2:36" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>23</v>
+      </c>
+      <c r="C26">
+        <v>286</v>
+      </c>
+      <c r="D26">
+        <v>159</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26" s="6">
+        <v>45887.504166666666</v>
+      </c>
+      <c r="H26" s="6">
+        <v>45890.406944444447</v>
+      </c>
+      <c r="I26">
+        <v>11.9</v>
+      </c>
+      <c r="J26">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="K26">
         <v>2.5</v>
       </c>
-      <c r="G30">
-        <f>(G28+G29)/2</f>
-        <v>29.334110460748349</v>
-      </c>
-      <c r="I30">
-        <v>1063</v>
-      </c>
-      <c r="J30">
-        <v>1.65</v>
-      </c>
-      <c r="K30">
-        <v>1.85</v>
-      </c>
-      <c r="L30">
-        <f t="shared" si="61"/>
-        <v>-0.20000000000000018</v>
-      </c>
-      <c r="M30">
-        <v>5679</v>
-      </c>
-      <c r="N30">
-        <v>10.45</v>
-      </c>
-      <c r="O30">
-        <v>9.86</v>
-      </c>
-      <c r="P30">
-        <f t="shared" si="62"/>
-        <v>0.58999999999999986</v>
-      </c>
-    </row>
-    <row r="31" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="G31">
-        <f>G30*F30</f>
-        <v>73.335276151870872</v>
-      </c>
-    </row>
-    <row r="33" spans="9:20" x14ac:dyDescent="0.35">
-      <c r="I33">
-        <f>247/-0.03</f>
-        <v>-8233.3333333333339</v>
-      </c>
-      <c r="M33">
-        <f>M28/P28</f>
-        <v>45566.666666666963</v>
-      </c>
-      <c r="Q33">
-        <f>Q28/T28</f>
-        <v>-11750.000000000022</v>
-      </c>
-    </row>
-    <row r="34" spans="9:20" x14ac:dyDescent="0.35">
-      <c r="I34">
-        <f>1063/-0.2</f>
-        <v>-5315</v>
-      </c>
-      <c r="M34">
-        <f t="shared" ref="M34:M35" si="63">M29/P29</f>
-        <v>7699.9999999999927</v>
-      </c>
-      <c r="Q34">
-        <f>Q29/T29</f>
-        <v>-11436.363636363649</v>
-      </c>
-    </row>
-    <row r="35" spans="9:20" x14ac:dyDescent="0.35">
-      <c r="M35">
-        <f t="shared" si="63"/>
-        <v>9625.423728813561</v>
-      </c>
-    </row>
-    <row r="37" spans="9:20" x14ac:dyDescent="0.35">
-      <c r="I37">
-        <f>5679/1063</f>
-        <v>5.3424270931326436</v>
-      </c>
-      <c r="Q37">
-        <f>M30/Q29</f>
-        <v>2.257154213036566</v>
-      </c>
-    </row>
-    <row r="38" spans="9:20" x14ac:dyDescent="0.35">
-      <c r="I38">
-        <f>I30*I37</f>
-        <v>5679</v>
-      </c>
-      <c r="L38">
-        <f>L30*I37</f>
-        <v>-1.0684854186265296</v>
-      </c>
-      <c r="Q38">
-        <f>Q29*Q37</f>
-        <v>5679</v>
-      </c>
-      <c r="T38">
-        <f>T29*Q37</f>
-        <v>-0.49657392686804397</v>
-      </c>
-    </row>
-    <row r="44" spans="9:20" x14ac:dyDescent="0.35">
-      <c r="I44">
-        <v>65.77</v>
-      </c>
-      <c r="K44">
-        <v>80.89</v>
-      </c>
-      <c r="M44">
-        <v>74</v>
-      </c>
-      <c r="O44">
-        <v>77.150000000000006</v>
-      </c>
-    </row>
-    <row r="45" spans="9:20" x14ac:dyDescent="0.35">
-      <c r="I45">
-        <f>L38</f>
-        <v>-1.0684854186265296</v>
-      </c>
-      <c r="K45">
-        <f>P30</f>
-        <v>0.58999999999999986</v>
-      </c>
-      <c r="M45">
-        <f>T38</f>
-        <v>-0.49657392686804397</v>
-      </c>
-      <c r="O45">
-        <v>0</v>
+      <c r="O26" s="3">
+        <f t="shared" ref="O26" si="76">H26-G26</f>
+        <v>2.9027777777810115</v>
+      </c>
+      <c r="P26" s="4">
+        <f t="shared" ref="P26" si="77">O26</f>
+        <v>2.9027777777810115</v>
+      </c>
+      <c r="Q26" s="5">
+        <f t="shared" ref="Q26" si="78">I26-J26</f>
+        <v>7</v>
+      </c>
+      <c r="R26" s="1">
+        <f t="shared" ref="R26" si="79">(F26-E26)/0.9982</f>
+        <v>0</v>
+      </c>
+      <c r="S26" s="5">
+        <f t="shared" ref="S26" si="80">K26*P26</f>
+        <v>7.2569444444525288</v>
+      </c>
+      <c r="U26" s="1">
+        <f>Q26*1440/4180</f>
+        <v>2.4114832535885169</v>
+      </c>
+      <c r="V26" s="7">
+        <f t="shared" ref="V26" si="81">(1-ABS(U26-K26)/K26)*100%</f>
+        <v>0.96459330143540678</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="V4:V22">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="V4:V26">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P4:P26">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>

</xml_diff>

<commit_message>
Added Measurements and minor bug fixes in Arduino
</commit_message>
<xml_diff>
--- a/Measurements.xlsx
+++ b/Measurements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Perfusion_System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F4B7CC-1304-4732-9C0D-4575162C0E9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7645421-55F0-49BB-A06B-124D27B65011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -277,8 +277,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5A39537A-AD85-40E4-8132-CD746B4A4B1E}" name="Table1" displayName="Table1" ref="B3:L30" totalsRowShown="0">
-  <autoFilter ref="B3:L30" xr:uid="{5A39537A-AD85-40E4-8132-CD746B4A4B1E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5A39537A-AD85-40E4-8132-CD746B4A4B1E}" name="Table1" displayName="Table1" ref="B3:L32" totalsRowShown="0">
+  <autoFilter ref="B3:L32" xr:uid="{5A39537A-AD85-40E4-8132-CD746B4A4B1E}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{7F49C8BC-1009-4421-9279-20BA630C3F5B}" name="Index"/>
     <tableColumn id="2" xr3:uid="{5E47D918-C96A-47BF-882D-1F6F0C3B3A06}" name="Raw_High"/>
@@ -596,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:AO30"/>
+  <dimension ref="B3:AO32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R36" sqref="R36"/>
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2476,18 +2476,181 @@
       </c>
     </row>
     <row r="30" spans="2:36" x14ac:dyDescent="0.35">
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="O30" s="3"/>
-      <c r="P30" s="4"/>
-      <c r="Q30" s="5"/>
-      <c r="R30" s="1"/>
-      <c r="S30" s="5"/>
-      <c r="U30" s="1"/>
-      <c r="V30" s="7"/>
+      <c r="B30">
+        <v>27</v>
+      </c>
+      <c r="E30">
+        <v>1408.7</v>
+      </c>
+      <c r="F30">
+        <v>1407.33</v>
+      </c>
+      <c r="G30" s="6">
+        <v>45894.666666666664</v>
+      </c>
+      <c r="H30" s="6">
+        <v>45895.46597222222</v>
+      </c>
+      <c r="I30">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="J30">
+        <v>8.5500000000000007</v>
+      </c>
+      <c r="K30">
+        <v>2.5</v>
+      </c>
+      <c r="O30" s="3">
+        <f t="shared" ref="O30:O31" si="94">H30-G30</f>
+        <v>0.79930555555620231</v>
+      </c>
+      <c r="P30" s="4">
+        <f t="shared" ref="P30:P31" si="95">O30</f>
+        <v>0.79930555555620231</v>
+      </c>
+      <c r="Q30" s="5">
+        <f t="shared" ref="Q30:Q31" si="96">I30-J30</f>
+        <v>1.1499999999999986</v>
+      </c>
+      <c r="R30" s="1">
+        <f t="shared" ref="R30:R31" si="97">(F30-E30)/0.9982</f>
+        <v>-1.372470446804366</v>
+      </c>
+      <c r="S30" s="5">
+        <f t="shared" ref="S30:S31" si="98">K30*P30</f>
+        <v>1.9982638888905058</v>
+      </c>
+      <c r="U30" s="1">
+        <f>Q30*1440/1151</f>
+        <v>1.4387489139878349</v>
+      </c>
+      <c r="V30" s="7">
+        <f t="shared" ref="V30:V31" si="99">(1-ABS(U30-K30)/K30)*100%</f>
+        <v>0.57549956559513393</v>
+      </c>
+    </row>
+    <row r="31" spans="2:36" x14ac:dyDescent="0.35">
+      <c r="B31">
+        <v>28</v>
+      </c>
+      <c r="C31">
+        <v>286</v>
+      </c>
+      <c r="D31">
+        <v>159</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31" s="6">
+        <v>45894.665277777778</v>
+      </c>
+      <c r="H31" s="6">
+        <v>45895.466666666667</v>
+      </c>
+      <c r="I31">
+        <v>11.5</v>
+      </c>
+      <c r="J31">
+        <v>9.9</v>
+      </c>
+      <c r="K31">
+        <v>2.5</v>
+      </c>
+      <c r="O31" s="3">
+        <f t="shared" si="94"/>
+        <v>0.80138888888905058</v>
+      </c>
+      <c r="P31" s="4">
+        <f t="shared" si="95"/>
+        <v>0.80138888888905058</v>
+      </c>
+      <c r="Q31" s="5">
+        <f t="shared" si="96"/>
+        <v>1.5999999999999996</v>
+      </c>
+      <c r="R31" s="1">
+        <f t="shared" si="97"/>
+        <v>0</v>
+      </c>
+      <c r="S31" s="5">
+        <f t="shared" si="98"/>
+        <v>2.0034722222226264</v>
+      </c>
+      <c r="U31" s="1">
+        <f>Q31*1440/1154</f>
+        <v>1.9965337954939337</v>
+      </c>
+      <c r="V31" s="7">
+        <f t="shared" si="99"/>
+        <v>0.79861351819757354</v>
+      </c>
+    </row>
+    <row r="32" spans="2:36" x14ac:dyDescent="0.35">
+      <c r="B32">
+        <v>29</v>
+      </c>
+      <c r="C32">
+        <v>286</v>
+      </c>
+      <c r="D32">
+        <v>159</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32" s="6">
+        <v>45895.534722222219</v>
+      </c>
+      <c r="H32" s="6">
+        <v>45895.573611111111</v>
+      </c>
+      <c r="I32">
+        <v>9.85</v>
+      </c>
+      <c r="J32">
+        <v>8.9</v>
+      </c>
+      <c r="K32">
+        <v>25</v>
+      </c>
+      <c r="O32" s="3">
+        <f t="shared" ref="O32" si="100">H32-G32</f>
+        <v>3.888888889196096E-2</v>
+      </c>
+      <c r="P32" s="4">
+        <f t="shared" ref="P32" si="101">O32</f>
+        <v>3.888888889196096E-2</v>
+      </c>
+      <c r="Q32" s="5">
+        <f t="shared" ref="Q32" si="102">I32-J32</f>
+        <v>0.94999999999999929</v>
+      </c>
+      <c r="R32" s="1">
+        <f t="shared" ref="R32" si="103">(F32-E32)/0.9982</f>
+        <v>0</v>
+      </c>
+      <c r="S32" s="5">
+        <f t="shared" ref="S32" si="104">K32*P32</f>
+        <v>0.972222222299024</v>
+      </c>
+      <c r="U32" s="1">
+        <f>Q32*1440/56</f>
+        <v>24.428571428571413</v>
+      </c>
+      <c r="V32" s="7">
+        <f t="shared" ref="V32" si="105">(1-ABS(U32-K32)/K32)*100%</f>
+        <v>0.97714285714285654</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="V4:V30">
+  <conditionalFormatting sqref="V4:V32">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2499,7 +2662,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P4:P30">
+  <conditionalFormatting sqref="P4:P32">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
New Measurements and 3D files for Gearbox added
</commit_message>
<xml_diff>
--- a/Measurements.xlsx
+++ b/Measurements.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Perfusion_System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E074384-77BE-4246-92C3-8FDDE9321185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC9DE8CA-3E26-4C95-B037-E052C422E910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>Raw_High</t>
   </si>
@@ -103,6 +104,45 @@
   </si>
   <si>
     <t>system 2</t>
+  </si>
+  <si>
+    <t>Perfusion No</t>
+  </si>
+  <si>
+    <t>Cornea No</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Pressure</t>
+  </si>
+  <si>
+    <t>Syringe Vol</t>
+  </si>
+  <si>
+    <t>Medium Perfused</t>
+  </si>
+  <si>
+    <t>Cornea Avg Thickness</t>
+  </si>
+  <si>
+    <t>avg</t>
+  </si>
+  <si>
+    <t>readings</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Total Duration</t>
+  </si>
+  <si>
+    <t>Change in Thickness</t>
+  </si>
+  <si>
+    <t>Total change in Thickness</t>
   </si>
 </sst>
 </file>
@@ -227,7 +267,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -241,6 +281,8 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="3"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
@@ -400,6 +442,23 @@
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{6AF60019-1C9C-460C-B40B-DFC95278CF4F}" name="Table8" displayName="Table8" ref="B2:I34" totalsRowShown="0">
+  <autoFilter ref="B2:I34" xr:uid="{6AF60019-1C9C-460C-B40B-DFC95278CF4F}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{57274A59-80BD-41BC-A570-03D4DC55F4DA}" name="Perfusion No"/>
+    <tableColumn id="2" xr3:uid="{1AC74BFE-39F5-4CB6-A7B1-C57D4BD339C0}" name="Cornea No"/>
+    <tableColumn id="3" xr3:uid="{0ED9A430-61F9-45C4-995E-D31D13FD2953}" name="Time"/>
+    <tableColumn id="4" xr3:uid="{923E45DE-2363-4AE8-8CCB-3F2F88D158D4}" name="Cornea Avg Thickness"/>
+    <tableColumn id="5" xr3:uid="{6E04E918-57C5-4616-A92F-D58E291FABD0}" name="Pressure"/>
+    <tableColumn id="6" xr3:uid="{084BA880-EC63-4B7D-853C-73E1D92AA904}" name="Syringe Vol"/>
+    <tableColumn id="7" xr3:uid="{751ADFA8-2474-48B3-91F3-F34D73DDF15F}" name="Medium Perfused"/>
+    <tableColumn id="8" xr3:uid="{4F622666-8BC8-40B5-B5FC-130C3FCC132D}" name="Duration"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -669,7 +728,7 @@
   <dimension ref="A3:AO54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I47" sqref="I47"/>
+      <selection activeCell="T54" sqref="T54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3723,40 +3782,454 @@
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
+      <c r="A47">
+        <v>44</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47" s="6">
+        <v>45909.593055555553</v>
+      </c>
+      <c r="G47" s="6">
+        <v>45910.438194444447</v>
+      </c>
+      <c r="H47">
+        <v>8.85</v>
+      </c>
+      <c r="I47">
+        <v>6.3</v>
+      </c>
+      <c r="J47">
+        <v>2.5</v>
+      </c>
+      <c r="K47" t="s">
+        <v>22</v>
+      </c>
+      <c r="N47" s="3">
+        <f t="shared" ref="N47" si="97">G47-F47</f>
+        <v>0.84513888889341615</v>
+      </c>
+      <c r="O47" s="4">
+        <f t="shared" ref="O47" si="98">N47</f>
+        <v>0.84513888889341615</v>
+      </c>
+      <c r="P47" s="5">
+        <f t="shared" ref="P47" si="99">H47-I47</f>
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="Q47" s="1">
+        <f t="shared" ref="Q47" si="100">ABS((E47-D47)/0.9982)</f>
+        <v>0</v>
+      </c>
+      <c r="R47" s="5">
+        <f t="shared" ref="R47" si="101">J47*O47</f>
+        <v>2.1128472222335404</v>
+      </c>
+      <c r="S47">
+        <f t="shared" ref="S47" si="102">(1-ABS(Q47-R47)/R47)*100</f>
+        <v>0</v>
+      </c>
+      <c r="T47" s="1">
+        <f>P47*1440/1217</f>
+        <v>3.0172555464256363</v>
+      </c>
+      <c r="U47" s="7">
+        <f t="shared" ref="U47" si="103">(1-ABS(T47-J47)/J47)*100%</f>
+        <v>0.79309778142974552</v>
+      </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="F48" s="6"/>
-      <c r="G48" s="6"/>
-    </row>
-    <row r="49" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F49" s="6"/>
-      <c r="G49" s="6"/>
-    </row>
-    <row r="50" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
-    </row>
-    <row r="51" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
-    </row>
-    <row r="52" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F52" s="6"/>
-      <c r="G52" s="6"/>
-    </row>
-    <row r="53" spans="6:7" x14ac:dyDescent="0.35">
-      <c r="F53" s="6"/>
-      <c r="G53" s="6"/>
-    </row>
-    <row r="54" spans="6:7" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>45</v>
+      </c>
+      <c r="B48">
+        <v>286</v>
+      </c>
+      <c r="C48">
+        <v>159</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48" s="6">
+        <v>45909.510416666664</v>
+      </c>
+      <c r="G48" s="6">
+        <v>45910.433333333334</v>
+      </c>
+      <c r="H48">
+        <v>10.7</v>
+      </c>
+      <c r="I48">
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="J48">
+        <v>2.5</v>
+      </c>
+      <c r="N48" s="3">
+        <f t="shared" ref="N48" si="104">G48-F48</f>
+        <v>0.92291666667006211</v>
+      </c>
+      <c r="O48" s="4">
+        <f t="shared" ref="O48" si="105">N48</f>
+        <v>0.92291666667006211</v>
+      </c>
+      <c r="P48" s="5">
+        <f t="shared" ref="P48" si="106">H48-I48</f>
+        <v>2.25</v>
+      </c>
+      <c r="Q48" s="1">
+        <f t="shared" ref="Q48" si="107">ABS((E48-D48)/0.9982)</f>
+        <v>0</v>
+      </c>
+      <c r="R48" s="5">
+        <f t="shared" ref="R48" si="108">J48*O48</f>
+        <v>2.3072916666751553</v>
+      </c>
+      <c r="S48">
+        <f t="shared" ref="S48" si="109">(1-ABS(Q48-R48)/R48)*100</f>
+        <v>0</v>
+      </c>
+      <c r="T48" s="1">
+        <f>P48*1440/1329</f>
+        <v>2.4379232505643342</v>
+      </c>
+      <c r="U48" s="7">
+        <f t="shared" ref="U48" si="110">(1-ABS(T48-J48)/J48)*100%</f>
+        <v>0.97516930022573367</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>46</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49" s="6">
+        <v>45910.463194444441</v>
+      </c>
+      <c r="G49" s="6">
+        <v>45912.175000000003</v>
+      </c>
+      <c r="H49">
+        <v>6.3</v>
+      </c>
+      <c r="I49">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="J49">
+        <v>2.5</v>
+      </c>
+      <c r="K49" t="s">
+        <v>22</v>
+      </c>
+      <c r="N49" s="3">
+        <f t="shared" ref="N49" si="111">G49-F49</f>
+        <v>1.7118055555620231</v>
+      </c>
+      <c r="O49" s="4">
+        <f t="shared" ref="O49" si="112">N49</f>
+        <v>1.7118055555620231</v>
+      </c>
+      <c r="P49" s="5">
+        <f t="shared" ref="P49" si="113">H49-I49</f>
+        <v>5.15</v>
+      </c>
+      <c r="Q49" s="1">
+        <f t="shared" ref="Q49" si="114">ABS((E49-D49)/0.9982)</f>
+        <v>0</v>
+      </c>
+      <c r="R49" s="5">
+        <f t="shared" ref="R49" si="115">J49*O49</f>
+        <v>4.2795138889050577</v>
+      </c>
+      <c r="S49">
+        <f t="shared" ref="S49" si="116">(1-ABS(Q49-R49)/R49)*100</f>
+        <v>0</v>
+      </c>
+      <c r="T49" s="1">
+        <f>P49*1440/2465</f>
+        <v>3.0085192697768766</v>
+      </c>
+      <c r="U49" s="7">
+        <f t="shared" ref="U49" si="117">(1-ABS(T49-J49)/J49)*100%</f>
+        <v>0.79659229208924942</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>47</v>
+      </c>
+      <c r="B50">
+        <v>286</v>
+      </c>
+      <c r="C50">
+        <v>159</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50" s="6">
+        <v>45912.517361111109</v>
+      </c>
+      <c r="G50" s="6">
+        <v>45915.452777777777</v>
+      </c>
+      <c r="H50">
+        <v>11.2</v>
+      </c>
+      <c r="I50">
+        <v>2.4</v>
+      </c>
+      <c r="J50">
+        <v>2.5</v>
+      </c>
+      <c r="N50" s="3">
+        <f t="shared" ref="N50" si="118">G50-F50</f>
+        <v>2.9354166666671517</v>
+      </c>
+      <c r="O50" s="4">
+        <f t="shared" ref="O50" si="119">N50</f>
+        <v>2.9354166666671517</v>
+      </c>
+      <c r="P50" s="5">
+        <f t="shared" ref="P50" si="120">H50-I50</f>
+        <v>8.7999999999999989</v>
+      </c>
+      <c r="Q50" s="1">
+        <f t="shared" ref="Q50" si="121">ABS((E50-D50)/0.9982)</f>
+        <v>0</v>
+      </c>
+      <c r="R50" s="5">
+        <f t="shared" ref="R50" si="122">J50*O50</f>
+        <v>7.3385416666678793</v>
+      </c>
+      <c r="S50">
+        <f t="shared" ref="S50" si="123">(1-ABS(Q50-R50)/R50)*100</f>
+        <v>0</v>
+      </c>
+      <c r="T50" s="1">
+        <f>P50*1440/4227</f>
+        <v>2.997870830376153</v>
+      </c>
+      <c r="U50" s="7">
+        <f t="shared" ref="U50" si="124">(1-ABS(T50-J50)/J50)*100%</f>
+        <v>0.80085166784953876</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>48</v>
+      </c>
+      <c r="B51">
+        <v>286</v>
+      </c>
+      <c r="C51">
+        <v>159</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51" s="6">
+        <v>45915.5625</v>
+      </c>
+      <c r="G51" s="6">
+        <v>45915.701388888891</v>
+      </c>
+      <c r="H51">
+        <v>11.7</v>
+      </c>
+      <c r="I51">
+        <v>11.3</v>
+      </c>
+      <c r="J51">
+        <v>2.5</v>
+      </c>
+      <c r="N51" s="3">
+        <f t="shared" ref="N51" si="125">G51-F51</f>
+        <v>0.13888888889050577</v>
+      </c>
+      <c r="O51" s="4">
+        <f t="shared" ref="O51" si="126">N51</f>
+        <v>0.13888888889050577</v>
+      </c>
+      <c r="P51" s="5">
+        <f t="shared" ref="P51" si="127">H51-I51</f>
+        <v>0.39999999999999858</v>
+      </c>
+      <c r="Q51" s="1">
+        <f t="shared" ref="Q51" si="128">ABS((E51-D51)/0.9982)</f>
+        <v>0</v>
+      </c>
+      <c r="R51" s="5">
+        <f t="shared" ref="R51" si="129">J51*O51</f>
+        <v>0.34722222222626442</v>
+      </c>
+      <c r="S51">
+        <f t="shared" ref="S51" si="130">(1-ABS(Q51-R51)/R51)*100</f>
+        <v>0</v>
+      </c>
+      <c r="T51" s="1">
+        <f>P51*1440/200</f>
+        <v>2.8799999999999897</v>
+      </c>
+      <c r="U51" s="7">
+        <f t="shared" ref="U51" si="131">(1-ABS(T51-J51)/J51)*100%</f>
+        <v>0.84800000000000408</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>49</v>
+      </c>
+      <c r="B52">
+        <v>286</v>
+      </c>
+      <c r="C52">
+        <v>159</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52" s="6">
+        <v>45915.5625</v>
+      </c>
+      <c r="G52" s="6">
+        <v>45916.452777777777</v>
+      </c>
+      <c r="H52">
+        <v>11.7</v>
+      </c>
+      <c r="I52">
+        <v>9.1</v>
+      </c>
+      <c r="J52">
+        <v>2.5</v>
+      </c>
+      <c r="N52" s="3">
+        <f t="shared" ref="N52" si="132">G52-F52</f>
+        <v>0.89027777777664596</v>
+      </c>
+      <c r="O52" s="4">
+        <f t="shared" ref="O52" si="133">N52</f>
+        <v>0.89027777777664596</v>
+      </c>
+      <c r="P52" s="5">
+        <f t="shared" ref="P52" si="134">H52-I52</f>
+        <v>2.5999999999999996</v>
+      </c>
+      <c r="Q52" s="1">
+        <f t="shared" ref="Q52" si="135">ABS((E52-D52)/0.9982)</f>
+        <v>0</v>
+      </c>
+      <c r="R52" s="5">
+        <f t="shared" ref="R52" si="136">J52*O52</f>
+        <v>2.2256944444416149</v>
+      </c>
+      <c r="S52">
+        <f t="shared" ref="S52" si="137">(1-ABS(Q52-R52)/R52)*100</f>
+        <v>0</v>
+      </c>
+      <c r="T52" s="1">
+        <f>P52*1440/1282</f>
+        <v>2.9204368174726985</v>
+      </c>
+      <c r="U52" s="7">
+        <f t="shared" ref="U52" si="138">(1-ABS(T52-J52)/J52)*100%</f>
+        <v>0.83182527301092057</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>50</v>
+      </c>
+      <c r="B53">
+        <v>286</v>
+      </c>
+      <c r="C53">
+        <v>159</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53" s="6">
+        <v>45915.5625</v>
+      </c>
+      <c r="G53" s="6">
+        <v>45916.731944444444</v>
+      </c>
+      <c r="H53">
+        <v>11.7</v>
+      </c>
+      <c r="I53">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="J53">
+        <v>2.5</v>
+      </c>
+      <c r="N53" s="3">
+        <f t="shared" ref="N53" si="139">G53-F53</f>
+        <v>1.1694444444437977</v>
+      </c>
+      <c r="O53" s="4">
+        <f t="shared" ref="O53" si="140">N53</f>
+        <v>1.1694444444437977</v>
+      </c>
+      <c r="P53" s="5">
+        <f t="shared" ref="P53" si="141">H53-I53</f>
+        <v>3.3999999999999986</v>
+      </c>
+      <c r="Q53" s="1">
+        <f t="shared" ref="Q53" si="142">ABS((E53-D53)/0.9982)</f>
+        <v>0</v>
+      </c>
+      <c r="R53" s="5">
+        <f t="shared" ref="R53" si="143">J53*O53</f>
+        <v>2.9236111111094942</v>
+      </c>
+      <c r="S53">
+        <f t="shared" ref="S53" si="144">(1-ABS(Q53-R53)/R53)*100</f>
+        <v>0</v>
+      </c>
+      <c r="T53" s="1">
+        <f>P53*1440/1684</f>
+        <v>2.9073634204275525</v>
+      </c>
+      <c r="U53" s="7">
+        <f t="shared" ref="U53" si="145">(1-ABS(T53-J53)/J53)*100%</f>
+        <v>0.83705463182897899</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.35">
       <c r="F54" s="6"/>
       <c r="G54" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
-  <conditionalFormatting sqref="U4:U46">
+  <conditionalFormatting sqref="U4:U53">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -3768,7 +4241,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O4:O46">
+  <conditionalFormatting sqref="O4:O53">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -3787,4 +4260,356 @@
     <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9C5FDAC-98D4-4D18-97AA-B3B6D97F2F65}">
+  <dimension ref="B2:W13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="13.54296875" customWidth="1"/>
+    <col min="3" max="3" width="11.6328125" customWidth="1"/>
+    <col min="4" max="4" width="14.6328125" customWidth="1"/>
+    <col min="5" max="5" width="20.7265625" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="11.90625" customWidth="1"/>
+    <col min="8" max="8" width="17.6328125" customWidth="1"/>
+    <col min="9" max="9" width="20.453125" customWidth="1"/>
+    <col min="11" max="11" width="13.6328125" customWidth="1"/>
+    <col min="12" max="12" width="18.6328125" customWidth="1"/>
+    <col min="13" max="13" width="18.90625" customWidth="1"/>
+    <col min="14" max="14" width="22.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="11">
+        <v>45903.534722222219</v>
+      </c>
+      <c r="E3">
+        <v>1001</v>
+      </c>
+      <c r="F3">
+        <v>15</v>
+      </c>
+      <c r="G3">
+        <v>11.7</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="11">
+        <v>45903.68472222222</v>
+      </c>
+      <c r="E4">
+        <v>982</v>
+      </c>
+      <c r="F4">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="3">
+        <f>D4-D3</f>
+        <v>0.15000000000145519</v>
+      </c>
+      <c r="V4" t="s">
+        <v>31</v>
+      </c>
+      <c r="W4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="11">
+        <v>45904.477777777778</v>
+      </c>
+      <c r="E5">
+        <v>887</v>
+      </c>
+      <c r="F5">
+        <v>15</v>
+      </c>
+      <c r="G5">
+        <v>9.4499999999999993</v>
+      </c>
+      <c r="H5">
+        <f>11.7-9.45</f>
+        <v>2.25</v>
+      </c>
+      <c r="I5" s="3">
+        <f>D5-D4</f>
+        <v>0.7930555555576575</v>
+      </c>
+      <c r="V5">
+        <v>777</v>
+      </c>
+      <c r="W5">
+        <f>AVERAGE(V5,V6,V7,V8,V9)</f>
+        <v>775.4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="11">
+        <v>45904.740277777775</v>
+      </c>
+      <c r="E6">
+        <v>893</v>
+      </c>
+      <c r="F6">
+        <v>15</v>
+      </c>
+      <c r="G6">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="H6">
+        <f>9.45-8.7</f>
+        <v>0.75</v>
+      </c>
+      <c r="I6" s="3">
+        <f>D6-D5</f>
+        <v>0.26249999999708962</v>
+      </c>
+      <c r="K6" t="s">
+        <v>33</v>
+      </c>
+      <c r="L6" t="s">
+        <v>28</v>
+      </c>
+      <c r="M6" t="s">
+        <v>34</v>
+      </c>
+      <c r="N6" t="s">
+        <v>35</v>
+      </c>
+      <c r="V6">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="7" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="11">
+        <v>45905.469444444447</v>
+      </c>
+      <c r="E7">
+        <v>843</v>
+      </c>
+      <c r="F7">
+        <v>15</v>
+      </c>
+      <c r="G7">
+        <v>7</v>
+      </c>
+      <c r="H7">
+        <f>8.7-7</f>
+        <v>1.6999999999999993</v>
+      </c>
+      <c r="I7" s="3">
+        <f>D7-D6</f>
+        <v>0.72916666667151731</v>
+      </c>
+      <c r="K7" s="12">
+        <f>SUM(I4,I5,I6,I7)</f>
+        <v>1.9347222222277196</v>
+      </c>
+      <c r="L7">
+        <f>11.7-7</f>
+        <v>4.6999999999999993</v>
+      </c>
+      <c r="M7">
+        <f>1001-843</f>
+        <v>158</v>
+      </c>
+      <c r="V7">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="8" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="V8">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="9" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="11">
+        <v>45905.501388888886</v>
+      </c>
+      <c r="E9">
+        <v>843</v>
+      </c>
+      <c r="F9">
+        <v>15</v>
+      </c>
+      <c r="G9">
+        <v>10.1</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="10" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" s="11">
+        <v>45905.72152777778</v>
+      </c>
+      <c r="E10">
+        <v>831</v>
+      </c>
+      <c r="F10">
+        <v>15</v>
+      </c>
+      <c r="G10">
+        <v>9.6</v>
+      </c>
+      <c r="H10">
+        <f>10.1-9.6</f>
+        <v>0.5</v>
+      </c>
+      <c r="I10" s="3">
+        <f>D10-D9</f>
+        <v>0.22013888889341615</v>
+      </c>
+    </row>
+    <row r="11" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" s="11">
+        <v>45908.460416666669</v>
+      </c>
+      <c r="E11">
+        <v>775</v>
+      </c>
+      <c r="F11">
+        <v>15</v>
+      </c>
+      <c r="G11">
+        <v>2.7</v>
+      </c>
+      <c r="H11">
+        <f>9.6-2.7</f>
+        <v>6.8999999999999995</v>
+      </c>
+      <c r="I11" s="3">
+        <f>D11-D10</f>
+        <v>2.7388888888890506</v>
+      </c>
+      <c r="K11" s="12">
+        <f>SUM(I10,I11)</f>
+        <v>2.9590277777824667</v>
+      </c>
+      <c r="L11">
+        <f>10.1-2.7</f>
+        <v>7.3999999999999995</v>
+      </c>
+      <c r="M11">
+        <f>843-775</f>
+        <v>68</v>
+      </c>
+      <c r="N11">
+        <f>1001-775</f>
+        <v>226</v>
+      </c>
+    </row>
+    <row r="13" spans="2:23" x14ac:dyDescent="0.35">
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Output file name changed for CSV files
</commit_message>
<xml_diff>
--- a/Measurements.xlsx
+++ b/Measurements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Perfusion_System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC9DE8CA-3E26-4C95-B037-E052C422E910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B707BCD2-91C4-4BC7-B368-521AAC19BB0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4224,12 +4224,66 @@
       </c>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="F54" s="6"/>
-      <c r="G54" s="6"/>
+      <c r="A54">
+        <v>51</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54" s="6">
+        <v>45918.588194444441</v>
+      </c>
+      <c r="G54" s="6">
+        <v>45922.322222222225</v>
+      </c>
+      <c r="H54">
+        <v>11.8</v>
+      </c>
+      <c r="I54">
+        <v>0.7</v>
+      </c>
+      <c r="J54">
+        <v>2.5</v>
+      </c>
+      <c r="N54" s="3">
+        <f t="shared" ref="N54" si="146">G54-F54</f>
+        <v>3.7340277777839219</v>
+      </c>
+      <c r="O54" s="4">
+        <f t="shared" ref="O54" si="147">N54</f>
+        <v>3.7340277777839219</v>
+      </c>
+      <c r="P54" s="5">
+        <f t="shared" ref="P54" si="148">H54-I54</f>
+        <v>11.100000000000001</v>
+      </c>
+      <c r="Q54" s="1">
+        <f t="shared" ref="Q54" si="149">ABS((E54-D54)/0.9982)</f>
+        <v>0</v>
+      </c>
+      <c r="R54" s="5">
+        <f t="shared" ref="R54" si="150">J54*O54</f>
+        <v>9.3350694444598048</v>
+      </c>
+      <c r="S54">
+        <f t="shared" ref="S54" si="151">(1-ABS(Q54-R54)/R54)*100</f>
+        <v>0</v>
+      </c>
+      <c r="T54" s="1">
+        <f>P54*1440/5377</f>
+        <v>2.9726613353170919</v>
+      </c>
+      <c r="U54" s="7">
+        <f t="shared" ref="U54" si="152">(1-ABS(T54-J54)/J54)*100%</f>
+        <v>0.81093546587316323</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
-  <conditionalFormatting sqref="U4:U53">
+  <conditionalFormatting sqref="U4:U54">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -4241,7 +4295,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O4:O53">
+  <conditionalFormatting sqref="O4:O54">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
New Measurements added to the Excel file
</commit_message>
<xml_diff>
--- a/Measurements.xlsx
+++ b/Measurements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Perfusion_System\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramza\Downloads\Perfusion_System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DCB79E0-90D0-40BD-A2B8-EFDB4E9F9ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF0653AE-4C5D-411F-9966-554B0AACE647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -439,8 +439,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5A39537A-AD85-40E4-8132-CD746B4A4B1E}" name="Table1" displayName="Table1" ref="A3:K65" totalsRowShown="0">
-  <autoFilter ref="A3:K65" xr:uid="{5A39537A-AD85-40E4-8132-CD746B4A4B1E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5A39537A-AD85-40E4-8132-CD746B4A4B1E}" name="Table1" displayName="Table1" ref="A3:K76" totalsRowShown="0">
+  <autoFilter ref="A3:K76" xr:uid="{5A39537A-AD85-40E4-8132-CD746B4A4B1E}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{7F49C8BC-1009-4421-9279-20BA630C3F5B}" name="Index"/>
     <tableColumn id="2" xr3:uid="{5E47D918-C96A-47BF-882D-1F6F0C3B3A06}" name="Raw_High"/>
@@ -787,38 +787,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:AO65"/>
+  <dimension ref="A3:AO78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J67" sqref="J67"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I66" sqref="I66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.1796875" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" customWidth="1"/>
-    <col min="3" max="3" width="11.08984375" customWidth="1"/>
-    <col min="4" max="4" width="15.36328125" customWidth="1"/>
-    <col min="5" max="5" width="14.08984375" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="17.7265625" customWidth="1"/>
-    <col min="8" max="8" width="19.26953125" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
-    <col min="10" max="10" width="20.26953125" customWidth="1"/>
-    <col min="11" max="11" width="20.54296875" customWidth="1"/>
-    <col min="12" max="12" width="13.36328125" customWidth="1"/>
-    <col min="14" max="14" width="10.453125" customWidth="1"/>
-    <col min="15" max="15" width="16.36328125" customWidth="1"/>
-    <col min="16" max="16" width="19.08984375" customWidth="1"/>
-    <col min="17" max="17" width="18.54296875" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" customWidth="1"/>
+    <col min="11" max="11" width="20.5703125" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" customWidth="1"/>
+    <col min="15" max="15" width="16.42578125" customWidth="1"/>
+    <col min="16" max="16" width="19.140625" customWidth="1"/>
+    <col min="17" max="17" width="18.5703125" customWidth="1"/>
     <col min="18" max="18" width="25" customWidth="1"/>
-    <col min="19" max="19" width="13.7265625" customWidth="1"/>
-    <col min="20" max="20" width="11.36328125" customWidth="1"/>
-    <col min="21" max="21" width="11.54296875" customWidth="1"/>
-    <col min="22" max="22" width="10.54296875" customWidth="1"/>
+    <col min="19" max="19" width="13.7109375" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" customWidth="1"/>
+    <col min="21" max="21" width="11.5703125" customWidth="1"/>
+    <col min="22" max="22" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -886,7 +886,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1002,7 +1002,7 @@
         <v>-7.9999999999999849E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1118,7 +1118,7 @@
         <v>-0.21999999999999975</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1215,7 +1215,7 @@
         <v>0.58999999999999986</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>73.335276151870872</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -1350,7 +1350,7 @@
         <v>0.89704918032786907</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -1429,7 +1429,7 @@
         <v>-11750.000000000022</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>-11436.363636363649</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>9625.423728813561</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>0.99914893617021305</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>2.257154213036566</v>
       </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11</v>
       </c>
@@ -1789,7 +1789,7 @@
         <v>-0.49657392686804397</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>0.98873445501097346</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>0.94009508716323309</v>
       </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>14</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>0.92467532467532454</v>
       </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>15</v>
       </c>
@@ -2048,7 +2048,7 @@
         <v>0.94978723404255361</v>
       </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>16</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>0.95007949125596203</v>
       </c>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>17</v>
       </c>
@@ -2191,7 +2191,7 @@
         <v>77.150000000000006</v>
       </c>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>18</v>
       </c>
@@ -2273,7 +2273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>19</v>
       </c>
@@ -2337,7 +2337,7 @@
         <v>0.96221198156682042</v>
       </c>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>0.95206611570247923</v>
       </c>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>21</v>
       </c>
@@ -2465,7 +2465,7 @@
         <v>0.97014531043593144</v>
       </c>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>22</v>
       </c>
@@ -2529,7 +2529,7 @@
         <v>0.94999999999999962</v>
       </c>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>23</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>0.96459330143540678</v>
       </c>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>24</v>
       </c>
@@ -2654,7 +2654,7 @@
         <v>0.5458680818802123</v>
       </c>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>25</v>
       </c>
@@ -2718,7 +2718,7 @@
         <v>0.89794676806083662</v>
       </c>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>26</v>
       </c>
@@ -2779,7 +2779,7 @@
         <v>0.61714285714285677</v>
       </c>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>27</v>
       </c>
@@ -2837,7 +2837,7 @@
         <v>0.57549956559513393</v>
       </c>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>28</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>0.79861351819757354</v>
       </c>
     </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>29</v>
       </c>
@@ -2965,7 +2965,7 @@
         <v>0.97714285714285654</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>30</v>
       </c>
@@ -3029,7 +3029,7 @@
         <v>0.97548387096774181</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>31</v>
       </c>
@@ -3090,7 +3090,7 @@
         <v>0.58029850746268641</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>32</v>
       </c>
@@ -3154,7 +3154,7 @@
         <v>0.97246753246753226</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>33</v>
       </c>
@@ -3218,7 +3218,7 @@
         <v>0.96248529065662503</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>34</v>
       </c>
@@ -3279,7 +3279,7 @@
         <v>0.57858662254786108</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>35</v>
       </c>
@@ -3340,7 +3340,7 @@
         <v>0.51548638132295732</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>36</v>
       </c>
@@ -3407,7 +3407,7 @@
         <v>0.98476130256086003</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>37</v>
       </c>
@@ -3471,7 +3471,7 @@
         <v>0.99539170506912433</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>38</v>
       </c>
@@ -3535,7 +3535,7 @@
         <v>0.9734627831715208</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>39</v>
       </c>
@@ -3596,7 +3596,7 @@
         <v>0.48578313253011995</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>40</v>
       </c>
@@ -3657,7 +3657,7 @@
         <v>0.51428571428571423</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>41</v>
       </c>
@@ -3721,7 +3721,7 @@
         <v>0.99967143862942964</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>42</v>
       </c>
@@ -3782,7 +3782,7 @@
         <v>0.96500000000000019</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>43</v>
       </c>
@@ -3843,7 +3843,7 @@
         <v>0.89136013686911897</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>44</v>
       </c>
@@ -3904,7 +3904,7 @@
         <v>0.79309778142974552</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>45</v>
       </c>
@@ -3968,7 +3968,7 @@
         <v>0.97516930022573367</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>46</v>
       </c>
@@ -4029,7 +4029,7 @@
         <v>0.79659229208924942</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>47</v>
       </c>
@@ -4093,7 +4093,7 @@
         <v>0.80085166784953876</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>48</v>
       </c>
@@ -4157,7 +4157,7 @@
         <v>0.84800000000000408</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>49</v>
       </c>
@@ -4221,7 +4221,7 @@
         <v>0.83182527301092057</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>50</v>
       </c>
@@ -4285,7 +4285,7 @@
         <v>0.83705463182897899</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>51</v>
       </c>
@@ -4343,7 +4343,7 @@
         <v>0.81093546587316323</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>52</v>
       </c>
@@ -4404,7 +4404,7 @@
         <v>0.99529411764705911</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>53</v>
       </c>
@@ -4465,7 +4465,7 @@
         <v>0.96114421930870075</v>
       </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>54</v>
       </c>
@@ -4526,7 +4526,7 @@
         <v>0.96507936507936498</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>55</v>
       </c>
@@ -4587,7 +4587,7 @@
         <v>0.956552962298025</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>56</v>
       </c>
@@ -4654,7 +4654,7 @@
         <v>0.88216216216216181</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>57</v>
       </c>
@@ -4721,7 +4721,7 @@
         <v>0.9805309734513219</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>58</v>
       </c>
@@ -4782,7 +4782,7 @@
         <v>0.98461538461538534</v>
       </c>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>59</v>
       </c>
@@ -4849,7 +4849,7 @@
         <v>0.92313043478260892</v>
       </c>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>60</v>
       </c>
@@ -4916,7 +4916,7 @@
         <v>0.97737556561085981</v>
       </c>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>61</v>
       </c>
@@ -4977,7 +4977,7 @@
         <v>0.98375933046821973</v>
       </c>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>62</v>
       </c>
@@ -4988,10 +4988,16 @@
         <v>0</v>
       </c>
       <c r="F65" s="6">
-        <v>45930.870138888888</v>
+        <v>45931.513888888891</v>
       </c>
       <c r="G65" s="6">
-        <v>45931.25277777778</v>
+        <v>45933.553472222222</v>
+      </c>
+      <c r="H65">
+        <v>12</v>
+      </c>
+      <c r="I65">
+        <v>7</v>
       </c>
       <c r="J65">
         <v>2.5</v>
@@ -5001,15 +5007,15 @@
       </c>
       <c r="N65" s="3">
         <f t="shared" ref="N65" si="202">G65-F65</f>
-        <v>0.38263888889196096</v>
+        <v>2.0395833333313931</v>
       </c>
       <c r="O65" s="4">
         <f t="shared" ref="O65" si="203">N65</f>
-        <v>0.38263888889196096</v>
+        <v>2.0395833333313931</v>
       </c>
       <c r="P65" s="5">
         <f t="shared" ref="P65" si="204">H65-I65</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q65" s="1">
         <f t="shared" ref="Q65" si="205">ABS((E65-D65)/0.9982)</f>
@@ -5017,41 +5023,518 @@
       </c>
       <c r="R65" s="5">
         <f t="shared" ref="R65" si="206">J65*O65</f>
-        <v>0.9565972222299024</v>
+        <v>5.0989583333284827</v>
       </c>
       <c r="S65">
         <f t="shared" ref="S65" si="207">(1-ABS(Q65-R65)/R65)*100</f>
         <v>0</v>
       </c>
       <c r="T65" s="1">
-        <f>P65*1440/4421</f>
-        <v>0</v>
+        <f>P65*1440/2937</f>
+        <v>2.4514811031664965</v>
       </c>
       <c r="U65" s="7">
         <f t="shared" ref="U65" si="208">(1-ABS(T65-J65)/J65)*100%</f>
-        <v>0</v>
+        <v>0.98059244126659861</v>
+      </c>
+    </row>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F66" s="6"/>
+      <c r="G66" s="6"/>
+      <c r="N66" s="3"/>
+      <c r="O66" s="4"/>
+      <c r="P66" s="5"/>
+      <c r="Q66" s="1"/>
+      <c r="R66" s="5"/>
+      <c r="T66" s="1"/>
+      <c r="U66" s="7"/>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F67" s="6"/>
+      <c r="G67" s="6"/>
+      <c r="N67" s="3"/>
+      <c r="O67" s="4"/>
+      <c r="P67" s="5"/>
+      <c r="Q67" s="1"/>
+      <c r="R67" s="5"/>
+      <c r="T67" s="1"/>
+      <c r="U67" s="7"/>
+    </row>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F68" s="6"/>
+      <c r="G68" s="6"/>
+      <c r="N68" s="3"/>
+      <c r="O68" s="4"/>
+      <c r="P68" s="5"/>
+      <c r="Q68" s="1"/>
+      <c r="R68" s="5"/>
+      <c r="T68" s="1"/>
+      <c r="U68" s="7"/>
+    </row>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F69" s="6"/>
+      <c r="G69" s="6"/>
+      <c r="N69" s="3"/>
+      <c r="O69" s="4"/>
+      <c r="P69" s="5"/>
+      <c r="Q69" s="1"/>
+      <c r="R69" s="5"/>
+      <c r="T69" s="1"/>
+      <c r="U69" s="7"/>
+    </row>
+    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F70" s="6"/>
+      <c r="G70" s="6"/>
+      <c r="N70" s="3"/>
+      <c r="O70" s="4"/>
+      <c r="P70" s="5"/>
+      <c r="Q70" s="1"/>
+      <c r="R70" s="5"/>
+      <c r="T70" s="1"/>
+      <c r="U70" s="7"/>
+    </row>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>1</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71" s="11">
+        <v>45903.534722222219</v>
+      </c>
+      <c r="G71" s="11">
+        <v>45905.469444444447</v>
+      </c>
+      <c r="H71">
+        <v>11.7</v>
+      </c>
+      <c r="I71">
+        <v>7</v>
+      </c>
+      <c r="J71">
+        <v>2.5</v>
+      </c>
+      <c r="N71" s="3">
+        <f t="shared" ref="N71" si="209">G71-F71</f>
+        <v>1.9347222222277196</v>
+      </c>
+      <c r="O71" s="4">
+        <f t="shared" ref="O71" si="210">N71</f>
+        <v>1.9347222222277196</v>
+      </c>
+      <c r="P71" s="5">
+        <f t="shared" ref="P71" si="211">H71-I71</f>
+        <v>4.6999999999999993</v>
+      </c>
+      <c r="Q71" s="1">
+        <f t="shared" ref="Q71" si="212">ABS((E71-D71)/0.9982)</f>
+        <v>0</v>
+      </c>
+      <c r="R71" s="5">
+        <f t="shared" ref="R71" si="213">J71*O71</f>
+        <v>4.836805555569299</v>
+      </c>
+      <c r="S71">
+        <f t="shared" ref="S71" si="214">(1-ABS(Q71-R71)/R71)*100</f>
+        <v>0</v>
+      </c>
+      <c r="T71" s="1">
+        <f>P71*1440/2786</f>
+        <v>2.4292893036611627</v>
+      </c>
+      <c r="U71" s="7">
+        <f t="shared" ref="U71" si="215">(1-ABS(T71-J71)/J71)*100%</f>
+        <v>0.97171572146446505</v>
+      </c>
+    </row>
+    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>1</v>
+      </c>
+      <c r="F72" s="11">
+        <v>45905.501388888886</v>
+      </c>
+      <c r="G72" s="11">
+        <v>45908.460416666669</v>
+      </c>
+      <c r="H72">
+        <v>10.1</v>
+      </c>
+      <c r="I72">
+        <v>2.7</v>
+      </c>
+      <c r="J72">
+        <v>2.5</v>
+      </c>
+      <c r="N72" s="3">
+        <f t="shared" ref="N72" si="216">G72-F72</f>
+        <v>2.9590277777824667</v>
+      </c>
+      <c r="O72" s="4">
+        <f t="shared" ref="O72" si="217">N72</f>
+        <v>2.9590277777824667</v>
+      </c>
+      <c r="P72" s="5">
+        <f t="shared" ref="P72" si="218">H72-I72</f>
+        <v>7.3999999999999995</v>
+      </c>
+      <c r="Q72" s="1">
+        <f t="shared" ref="Q72" si="219">ABS((E72-D72)/0.9982)</f>
+        <v>0</v>
+      </c>
+      <c r="R72" s="5">
+        <f t="shared" ref="R72" si="220">J72*O72</f>
+        <v>7.3975694444561668</v>
+      </c>
+      <c r="S72">
+        <f t="shared" ref="S72" si="221">(1-ABS(Q72-R72)/R72)*100</f>
+        <v>0</v>
+      </c>
+      <c r="T72" s="1">
+        <f>P72*1440/4261</f>
+        <v>2.5008214034264258</v>
+      </c>
+      <c r="U72" s="7">
+        <f t="shared" ref="U72" si="222">(1-ABS(T72-J72)/J72)*100%</f>
+        <v>0.99967143862942964</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>2</v>
+      </c>
+      <c r="F73" s="11">
+        <v>45909.48541666667</v>
+      </c>
+      <c r="G73" s="11">
+        <v>45911.393750000003</v>
+      </c>
+      <c r="H73">
+        <v>10.7</v>
+      </c>
+      <c r="I73">
+        <v>6</v>
+      </c>
+      <c r="J73">
+        <v>2.5</v>
+      </c>
+      <c r="N73" s="3">
+        <f t="shared" ref="N73" si="223">G73-F73</f>
+        <v>1.9083333333328483</v>
+      </c>
+      <c r="O73" s="4">
+        <f t="shared" ref="O73" si="224">N73</f>
+        <v>1.9083333333328483</v>
+      </c>
+      <c r="P73" s="5">
+        <f t="shared" ref="P73" si="225">H73-I73</f>
+        <v>4.6999999999999993</v>
+      </c>
+      <c r="Q73" s="1">
+        <f t="shared" ref="Q73" si="226">ABS((E73-D73)/0.9982)</f>
+        <v>0</v>
+      </c>
+      <c r="R73" s="5">
+        <f t="shared" ref="R73" si="227">J73*O73</f>
+        <v>4.7708333333321207</v>
+      </c>
+      <c r="S73">
+        <f t="shared" ref="S73" si="228">(1-ABS(Q73-R73)/R73)*100</f>
+        <v>0</v>
+      </c>
+      <c r="T73" s="1">
+        <f>P73*1440/2748</f>
+        <v>2.4628820960698685</v>
+      </c>
+      <c r="U73" s="7">
+        <f t="shared" ref="U73" si="229">(1-ABS(T73-J73)/J73)*100%</f>
+        <v>0.98515283842794743</v>
+      </c>
+    </row>
+    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>3</v>
+      </c>
+      <c r="F74" s="11">
+        <v>45912.517361111109</v>
+      </c>
+      <c r="G74" s="11">
+        <v>45915.452777777777</v>
+      </c>
+      <c r="H74">
+        <v>11.2</v>
+      </c>
+      <c r="I74">
+        <v>2.4</v>
+      </c>
+      <c r="J74">
+        <v>2.5</v>
+      </c>
+      <c r="N74" s="3">
+        <f t="shared" ref="N74" si="230">G74-F74</f>
+        <v>2.9354166666671517</v>
+      </c>
+      <c r="O74" s="4">
+        <f t="shared" ref="O74" si="231">N74</f>
+        <v>2.9354166666671517</v>
+      </c>
+      <c r="P74" s="5">
+        <f t="shared" ref="P74" si="232">H74-I74</f>
+        <v>8.7999999999999989</v>
+      </c>
+      <c r="Q74" s="1">
+        <f t="shared" ref="Q74" si="233">ABS((E74-D74)/0.9982)</f>
+        <v>0</v>
+      </c>
+      <c r="R74" s="5">
+        <f t="shared" ref="R74" si="234">J74*O74</f>
+        <v>7.3385416666678793</v>
+      </c>
+      <c r="S74">
+        <f t="shared" ref="S74" si="235">(1-ABS(Q74-R74)/R74)*100</f>
+        <v>0</v>
+      </c>
+      <c r="T74" s="1">
+        <f>P74*1440/4227</f>
+        <v>2.997870830376153</v>
+      </c>
+      <c r="U74" s="7">
+        <f t="shared" ref="U74" si="236">(1-ABS(T74-J74)/J74)*100%</f>
+        <v>0.80085166784953876</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>3</v>
+      </c>
+      <c r="F75" s="11">
+        <v>45915.701388888891</v>
+      </c>
+      <c r="G75" s="11">
+        <v>45916.731944444444</v>
+      </c>
+      <c r="H75">
+        <v>11.3</v>
+      </c>
+      <c r="I75">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="J75">
+        <v>2.5</v>
+      </c>
+      <c r="N75" s="3">
+        <f t="shared" ref="N75:N76" si="237">G75-F75</f>
+        <v>1.0305555555532919</v>
+      </c>
+      <c r="O75" s="4">
+        <f t="shared" ref="O75:O76" si="238">N75</f>
+        <v>1.0305555555532919</v>
+      </c>
+      <c r="P75" s="5">
+        <f t="shared" ref="P75:P76" si="239">H75-I75</f>
+        <v>3</v>
+      </c>
+      <c r="Q75" s="1">
+        <f t="shared" ref="Q75:Q76" si="240">ABS((E75-D75)/0.9982)</f>
+        <v>0</v>
+      </c>
+      <c r="R75" s="5">
+        <f t="shared" ref="R75:R76" si="241">J75*O75</f>
+        <v>2.5763888888832298</v>
+      </c>
+      <c r="S75">
+        <f t="shared" ref="S75:S76" si="242">(1-ABS(Q75-R75)/R75)*100</f>
+        <v>0</v>
+      </c>
+      <c r="T75" s="1">
+        <f>P75*1440/1484</f>
+        <v>2.9110512129380055</v>
+      </c>
+      <c r="U75" s="7">
+        <f t="shared" ref="U75:U76" si="243">(1-ABS(T75-J75)/J75)*100%</f>
+        <v>0.83557951482479775</v>
+      </c>
+    </row>
+    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>3</v>
+      </c>
+      <c r="F76" s="11">
+        <v>45919.415972222225</v>
+      </c>
+      <c r="G76" s="11">
+        <v>45920.629166666666</v>
+      </c>
+      <c r="H76">
+        <v>11.6</v>
+      </c>
+      <c r="I76">
+        <v>7.5</v>
+      </c>
+      <c r="J76">
+        <v>2.5</v>
+      </c>
+      <c r="N76" s="3">
+        <f t="shared" si="237"/>
+        <v>1.2131944444408873</v>
+      </c>
+      <c r="O76" s="4">
+        <f t="shared" si="238"/>
+        <v>1.2131944444408873</v>
+      </c>
+      <c r="P76" s="5">
+        <f t="shared" si="239"/>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="Q76" s="1">
+        <f t="shared" si="240"/>
+        <v>0</v>
+      </c>
+      <c r="R76" s="5">
+        <f t="shared" si="241"/>
+        <v>3.0329861111022183</v>
+      </c>
+      <c r="S76">
+        <f t="shared" si="242"/>
+        <v>0</v>
+      </c>
+      <c r="T76" s="1">
+        <f>P76*1440/1747</f>
+        <v>3.3795077275329128</v>
+      </c>
+      <c r="U76" s="7">
+        <f t="shared" si="243"/>
+        <v>0.64819690898683491</v>
+      </c>
+    </row>
+    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>4</v>
+      </c>
+      <c r="F77" s="11">
+        <v>45919.415972222225</v>
+      </c>
+      <c r="G77" s="11">
+        <v>45922.427777777775</v>
+      </c>
+      <c r="H77">
+        <v>11.6</v>
+      </c>
+      <c r="I77">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="J77">
+        <v>2.5</v>
+      </c>
+      <c r="N77" s="3">
+        <f t="shared" ref="N77" si="244">G77-F77</f>
+        <v>3.0118055555503815</v>
+      </c>
+      <c r="O77" s="4">
+        <f t="shared" ref="O77" si="245">N77</f>
+        <v>3.0118055555503815</v>
+      </c>
+      <c r="P77" s="5">
+        <f t="shared" ref="P77" si="246">H77-I77</f>
+        <v>9.3999999999999986</v>
+      </c>
+      <c r="Q77" s="1">
+        <f t="shared" ref="Q77" si="247">ABS((E77-D77)/0.9982)</f>
+        <v>0</v>
+      </c>
+      <c r="R77" s="5">
+        <f t="shared" ref="R77" si="248">J77*O77</f>
+        <v>7.5295138888759539</v>
+      </c>
+      <c r="S77">
+        <f t="shared" ref="S77" si="249">(1-ABS(Q77-R77)/R77)*100</f>
+        <v>0</v>
+      </c>
+      <c r="T77" s="1">
+        <f>P77*1440/4337</f>
+        <v>3.1210514180308966</v>
+      </c>
+      <c r="U77" s="7">
+        <f t="shared" ref="U77" si="250">(1-ABS(T77-J77)/J77)*100%</f>
+        <v>0.75157943278764139</v>
+      </c>
+    </row>
+    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>5</v>
+      </c>
+      <c r="F78" s="11">
+        <v>45930.557638888888</v>
+      </c>
+      <c r="G78" s="11">
+        <v>45930.695138888892</v>
+      </c>
+      <c r="H78">
+        <v>9.75</v>
+      </c>
+      <c r="I78">
+        <v>9.5</v>
+      </c>
+      <c r="J78">
+        <v>2.5</v>
+      </c>
+      <c r="N78" s="3">
+        <f t="shared" ref="N78" si="251">G78-F78</f>
+        <v>0.13750000000436557</v>
+      </c>
+      <c r="O78" s="4">
+        <f t="shared" ref="O78" si="252">N78</f>
+        <v>0.13750000000436557</v>
+      </c>
+      <c r="P78" s="5">
+        <f t="shared" ref="P78" si="253">H78-I78</f>
+        <v>0.25</v>
+      </c>
+      <c r="Q78" s="1">
+        <f t="shared" ref="Q78" si="254">ABS((E78-D78)/0.9982)</f>
+        <v>0</v>
+      </c>
+      <c r="R78" s="5">
+        <f t="shared" ref="R78" si="255">J78*O78</f>
+        <v>0.34375000001091394</v>
+      </c>
+      <c r="S78">
+        <f t="shared" ref="S78" si="256">(1-ABS(Q78-R78)/R78)*100</f>
+        <v>0</v>
+      </c>
+      <c r="T78" s="1">
+        <f>P78*1440/198</f>
+        <v>1.8181818181818181</v>
+      </c>
+      <c r="U78" s="7">
+        <f t="shared" ref="U78" si="257">(1-ABS(T78-J78)/J78)*100%</f>
+        <v>0.72727272727272729</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
-  <conditionalFormatting sqref="U4:U65">
-    <cfRule type="colorScale" priority="3">
+  <conditionalFormatting sqref="O4:O78">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U4:U78">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O4:O65">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
@@ -5072,26 +5555,26 @@
   <dimension ref="B2:W21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.54296875" customWidth="1"/>
-    <col min="3" max="3" width="11.6328125" customWidth="1"/>
-    <col min="4" max="4" width="14.6328125" customWidth="1"/>
-    <col min="5" max="5" width="20.7265625" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="11.90625" customWidth="1"/>
-    <col min="8" max="8" width="17.6328125" customWidth="1"/>
-    <col min="9" max="9" width="20.453125" customWidth="1"/>
-    <col min="11" max="11" width="13.6328125" customWidth="1"/>
-    <col min="12" max="12" width="18.6328125" customWidth="1"/>
-    <col min="13" max="13" width="18.90625" customWidth="1"/>
-    <col min="14" max="14" width="28.1796875" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" customWidth="1"/>
+    <col min="12" max="12" width="18.5703125" customWidth="1"/>
+    <col min="13" max="13" width="18.85546875" customWidth="1"/>
+    <col min="14" max="14" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>23</v>
       </c>
@@ -5117,7 +5600,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1</v>
       </c>
@@ -5143,7 +5626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
@@ -5176,7 +5659,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>1</v>
       </c>
@@ -5211,7 +5694,7 @@
         <v>807.6</v>
       </c>
     </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>1</v>
       </c>
@@ -5254,7 +5737,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>1</v>
       </c>
@@ -5297,12 +5780,12 @@
         <v>799</v>
       </c>
     </row>
-    <row r="8" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:23" x14ac:dyDescent="0.25">
       <c r="V8">
         <v>817</v>
       </c>
     </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>2</v>
       </c>
@@ -5331,7 +5814,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>2</v>
       </c>
@@ -5359,7 +5842,7 @@
         <v>0.22013888889341615</v>
       </c>
     </row>
-    <row r="11" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>2</v>
       </c>
@@ -5403,7 +5886,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>3</v>
       </c>
@@ -5423,7 +5906,7 @@
         <v>10.7</v>
       </c>
     </row>
-    <row r="14" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>3</v>
       </c>
@@ -5458,7 +5941,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="2:23" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>3</v>
       </c>
@@ -5502,7 +5985,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>4</v>
       </c>
@@ -5523,7 +6006,7 @@
       </c>
       <c r="K17" s="13"/>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>4</v>
       </c>
@@ -5555,7 +6038,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>5</v>
       </c>
@@ -5585,7 +6068,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>5</v>
       </c>
@@ -5620,7 +6103,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>5</v>
       </c>

</xml_diff>